<commit_message>
PGD Works; Improved data collection; Full Graph PGD is buggy
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,44 +367,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>epochs</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>epochs</t>
+          <t>op_reg</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>op_reg</t>
+          <t>learning_rate</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>learning_rate</t>
+          <t>adv_train_flag</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>adv_train_flag</t>
+          <t>activation</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>activation</t>
+          <t>acc_reg</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>acc_reg</t>
+          <t>acc_fgsm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>acc_robust</t>
+          <t>acc_pgd</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -414,190 +419,753 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>loss_robust</t>
+          <t>loss_pgd</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>loss_fgsm</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>logdir</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>weights_path</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>tb_dir</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Distances</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Norms</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>250</v>
+        <v>0.0007</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="E2" t="n">
         <v>0.0003</v>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Sigmoid</t>
         </is>
       </c>
+      <c r="G2" t="n">
+        <v>93.09999999999999</v>
+      </c>
       <c r="H2" t="n">
-        <v>93.09999999999999</v>
-      </c>
-      <c r="I2" t="n">
         <v>67.59999999999999</v>
       </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
         <v>0.2</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="n">
         <v>0.8</v>
       </c>
-      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
         <v>0.003</v>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
+      <c r="G3" t="n">
+        <v>0.7243999838829041</v>
+      </c>
       <c r="H3" t="n">
-        <v>0.7243999838829041</v>
-      </c>
-      <c r="I3" t="n">
         <v>0.05319999903440475</v>
       </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
         <v>0.8155719041824341</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="n">
         <v>5.454379558563232</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>logs/results_11.log</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
         <is>
           <t>tb/11/non_robust</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
         <v>0.003</v>
       </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
+      <c r="G4" t="n">
+        <v>0.7918999791145325</v>
+      </c>
       <c r="H4" t="n">
-        <v>0.7918999791145325</v>
-      </c>
-      <c r="I4" t="n">
         <v>0.05810000002384186</v>
       </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
         <v>0.6927952170372009</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
         <v>4.691385269165039</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>logs/results_13.log</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
         <is>
           <t>tb/13/non_robust</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>(0.9306673, 0.6533018, 0.6531849, 0.6674277, 0.6947321, 0.75724566, 0.7961144)</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>(&lt;tf.Tensor 'model_non_robust/Max_8:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_9:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_10:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_11:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_12:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_13:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_14:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_15:0' shape=() dtype=float32&gt;)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>sigmoid</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9466999769210815</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.1215000003576279</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>0.2134527862071991</v>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>6.628881454467773</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>logs/results_41.log</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>tb/41/non_robust</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>(0.9239762, 0.65693253, 0.6067492, 0.6374461, 0.64722586, 0.750713, 0.7882854)</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>(319.44058, 36.396854, 20.660694, 23.362183, 24.99871, 29.359327, 33.84145, 27.05041)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>sigmoid</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0.9369000196456909</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1234000027179718</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>0.2546896040439606</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>6.354927062988281</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>logs/results_42.log</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>tb/42/non_robust</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>(0.9097431, 0.59459233, 0.6237213, 0.646627, 0.70321494, 0.7542059, 0.80426776)</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>(325.33728, 32.12922, 22.591274, 19.652607, 20.43904, 26.104446, 38.55416, 27.83214)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>sigmoid</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0.9275000095367432</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.0681999996304512</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>0.297708123922348</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>7.019247531890869</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>logs/results_43.log</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>tb/43/non_robust</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>(0.8931245, 0.56005055, 0.59760016, 0.57427925, 0.6759137, 0.76545215, 0.78780127)</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>(326.3446, 31.664152, 22.359634, 21.57176, 27.57798, 34.183285, 35.271046, 29.007282)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>sigmoid</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0.944100022315979</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.01999999955296516</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>0.246184840798378</v>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>8.873349189758301</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>logs/results_44.log</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>tb/44/non_robust</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>(0.938725, 0.6600768, 0.66170657, 0.6852295, 0.7025278, 0.7467286, 0.76420873)</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>(329.55527, 26.631884, 20.483023, 21.433125, 23.539381, 28.294022, 27.846375, 27.025381)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>sigmoid</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0.9415000081062317</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.2319000065326691</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>0.2557807564735413</v>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>5.129439353942871</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>logs/results_45.log</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>tb/45/non_robust</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>(0.92154706, 0.6415282, 0.6576658, 0.6670158, 0.700283, 0.7661101, 0.80726135)</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>(332.50662, 27.713497, 22.988976, 24.210987, 22.345839, 28.06629, 34.470566, 28.11802)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Relu</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9623000025749207</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.03970000147819519</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>0.1634003221988678</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>8.993168830871582</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>logs/results_46.log</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>tb/46/non_robust</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>(13.717814, 18.26012, 24.893442, 31.145538, 29.057154, 20.91586, 15.984089)</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>(267.34714, 12.150078, 13.141031, 13.2189455, 9.97285, 8.843685, 8.705187, 13.771522)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Relu</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9621999859809875</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.06289999932050705</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>0.1620544195175171</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>28.44748115539551</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>logs/results_47.log</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>tb/47/non_robust</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>(13.70231, 18.81006, 24.938885, 29.81304, 33.936825, 19.185276, 17.508503)</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>(281.3783, 12.946939, 12.665519, 12.067004, 9.140996, 9.732248, 8.472949, 14.707483)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Relu</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.9298999905586243</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.03920000046491623</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.006000000052154064</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.2370504885911942</v>
+      </c>
+      <c r="K12" t="n">
+        <v>6.775509357452393</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.03920000046491623</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>logs/results_57.log</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>weights/model_57.ckpt</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>tb/57/non_robust</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>(7.4477954, 6.8025093, 7.2666335, 7.3556733, 8.691928, 8.399956, 8.053249)</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>(138.91463, 9.132495, 8.988977, 8.27085, 8.298483, 7.1643567, 7.5375657, 11.348869)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x117e589d8&gt;</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0.9531000256538391</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.04850000143051147</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.01339999958872795</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.1710376739501953</v>
+      </c>
+      <c r="K13" t="n">
+        <v>6.398704528808594</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.04850000143051147</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>logs/results_58.log</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>weights/model_58.ckpt</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>tb/58/non_robust</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>(7.135254, 7.887454, 7.845998, 8.052931, 8.5888, 8.207241, 6.9763064)</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>(140.55019, 9.100359, 9.088696, 8.028114, 8.66318, 7.551326, 7.209709, 10.0992565)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Altered scripts to generate histograms for final activations
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1169,6 +1169,274 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>30</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11ad159d8&gt;</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9657999873161316</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.2011000066995621</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.1811999976634979</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.1451183259487152</v>
+      </c>
+      <c r="K14" t="n">
+        <v>5.327450752258301</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.2011000066995621</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>logs/results_71.log</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>weights/model_71.ckpt</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>tb/71/non_robust</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>(5.475276, 12.719564, 18.869154, 27.198263, 26.215324, 22.13533, 16.86695)</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>(78.487724, 11.971958, 8.304008, 4.5321946, 2.381914, 1.7097418, 1.7520251, 2.2926486)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>30</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x12008f9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0.9585999846458435</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.2369000017642975</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.03700000047683716</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.1429557055234909</v>
+      </c>
+      <c r="K15" t="n">
+        <v>4.122503280639648</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.2369000017642975</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>logs/results_72.log</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>weights/model_72.ckpt</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>tb/72/non_robust</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>(2.139943, 3.496155, 3.843952, 5.1138744, 6.2203045, 6.9547405, 8.452685)</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>(29.190838, 5.508862, 3.9576876, 1.9097207, 1.488211, 1.3313731, 1.552425, 1.4604229)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>70</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1240199d8&gt;</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.9384999871253967</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.2345000058412552</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.07829999923706055</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.2154168486595154</v>
+      </c>
+      <c r="K16" t="n">
+        <v>4.516582012176514</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.2345000058412552</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>logs/results_74.log</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>weights/model_74.ckpt</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>tb/74/non_robust</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>(1.7076006, 2.5921235, 2.5732467, 3.4120953, 4.31576, 5.6463065, 6.7571893)</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>(23.436884, 4.6997, 2.8007762, 1.6223694, 1.4685857, 1.5694603, 1.4128212, 1.4283097)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>30</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>FGSM</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11951f9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0.9517999887466431</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8098999857902527</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4519999921321869</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.1830078810453415</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.6702156066894531</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.8098999857902527</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>logs/results_75.log</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>weights/model_75.ckpt</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>tb/75/robust</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>(6.767173, 17.473831, 38.257633, 49.1879, 27.285254, 10.4143715, 4.247443)</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>(131.64798, 17.081043, 17.57381, 15.574147, 13.246862, 13.433027, 11.568809, 11.362484)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Training works but some bug in FGSM gradients I think
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1437,6 +1437,274 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11e35f9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.009425175376236439</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.05570029467344284</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>logs/results_86.log</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>weights/model_86.ckpt</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>tb/86/non_robust</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>(0.06946261, 0.12680605, 0.10363617)</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>(117.439575, 8.788963, 6.8641105, 3.1679692)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x123bb89d8&gt;</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.00775056378915906</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.1920228749513626</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>logs/results_87.log</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>weights/model_87.ckpt</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>tb/87/non_robust</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>(0.18897994, 0.41342703, 0.28442824)</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>(109.61839, 8.210519, 6.61972, 2.5461638)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1170ae9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.00669969292357564</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.05489230528473854</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>logs/results_88.log</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>weights/model_88.ckpt</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>tb/88/non_robust</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>(0.05377488, 0.06494685, 0.081667334)</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>(107.84222, 7.0260696, 6.7622585, 3.9107814)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1191959d8&gt;</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.005836887285113335</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.03965282067656517</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>logs/results_90.log</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>weights/model_90.ckpt</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>tb/90/non_robust</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>(0.052884344, 0.08614982, 0.049282983)</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>(112.28816, 7.4369655, 6.118991, 3.4870443)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Geometric margin expt done and very weird PGD adv train implementation
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,6 +1705,1748 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1234d59d8&gt;</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.007372809108346701</v>
+      </c>
+      <c r="K22" t="n">
+        <v>11.56273460388184</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>logs/results_98.log</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>weights/model_98.ckpt</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>tb/98/non_robust</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>(4.5611963, 6.1438217, 6.2704434)</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>(84.79397, 6.59225, 7.4339743, 4.3686156)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x111d0c9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.007391395047307014</v>
+      </c>
+      <c r="K23" t="n">
+        <v>7.413827896118164</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>logs/results_99.log</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>weights/model_99.ckpt</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>tb/99/non_robust</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>(4.965393, 5.580272, 4.0586343)</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>(82.53853, 6.6707835, 6.1323104, 5.402368)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10bf399d8&gt;</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.01620800234377384</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.05398423597216606</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>logs/results_102.log</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>weights/model_102.ckpt</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>tb/102/non_robust</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>(4.6686077, 3.5514605, 1.5891917)</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>(106.69825, 6.9493837, 6.7535663, 3.6396196)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x116b9d9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.0161934494972229</v>
+      </c>
+      <c r="K25" t="n">
+        <v>7.627745151519775</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>logs/results_105.log</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>weights/model_105.ckpt</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>tb/105/non_robust</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>(5.317512, 6.190056, 4.687)</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>(84.34224, 6.941453, 6.490801, 4.822403)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>10</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1287c69d8&gt;</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.01950065977871418</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.06105006858706474</v>
+      </c>
+      <c r="L26" t="n">
+        <v>1</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>logs/results_106.log</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>weights/model_106.ckpt</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>tb/106/non_robust</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>(4.5039525, 4.046463, 1.6872294)</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>(106.4445, 8.165542, 6.774193, 3.1399925)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>10</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1248b39d8&gt;</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.008060908876359463</v>
+      </c>
+      <c r="K27" t="n">
+        <v>6.071034908294678</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>logs/results_107.log</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>weights/model_107.ckpt</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>tb/107/non_robust</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>(5.3797283, 5.525841, 4.273903)</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>(83.57327, 6.976924, 6.5643578, 5.417325)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11a4509d8&gt;</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.01825481466948986</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.05136026069521904</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>logs/results_108.log</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>weights/model_108.ckpt</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>tb/108/non_robust</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>(4.0847874, 3.4897168, 1.4608247)</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>(103.926285, 6.471912, 6.30821, 4.8110895)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>10</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1118429d8&gt;</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.007533956784754992</v>
+      </c>
+      <c r="K29" t="n">
+        <v>8.43317985534668</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>logs/results_109.log</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>weights/model_109.ckpt</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>tb/109/non_robust</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>(4.852438, 4.0877357, 4.599871)</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>(85.2768, 6.536387, 6.6221027, 5.935522)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>10</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x118f9b9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.01898444443941116</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.05481623858213425</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>logs/results_110.log</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>weights/model_110.ckpt</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>tb/110/non_robust</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>(4.2600565, 3.2923791, 1.4908074)</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>(107.223724, 7.3879747, 6.3947926, 5.007269)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>10</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1263589d8&gt;</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.01013232953846455</v>
+      </c>
+      <c r="K31" t="n">
+        <v>8.253989219665527</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>logs/results_111.log</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>weights/model_111.ckpt</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>tb/111/non_robust</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>(5.946497, 7.091279, 7.1287503)</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>(88.84125, 6.8087015, 6.36443, 4.6299343)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>10</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3e-07</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x122a009d8&gt;</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.8840473890304565</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1.409839749336243</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>logs/results_112.log</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>weights/model_112.ckpt</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>tb/112/non_robust</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>(1.4278239, 0.92267954, 0.5387663)</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>(35.329483, 5.654189, 6.8145466, 7.97134)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>10</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1255e49d8&gt;</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1.156007528305054</v>
+      </c>
+      <c r="K33" t="n">
+        <v>2.298643112182617</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>logs/results_113.log</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>weights/model_113.ckpt</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>tb/113/non_robust</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>(5.7392573, 5.4852233, 4.945301)</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>(82.004486, 6.780108, 6.6321454, 4.495418)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>10</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1236119d8&gt;</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>0.995356023311615</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.2832817435264587</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.04024767875671387</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.009356297552585602</v>
+      </c>
+      <c r="K34" t="n">
+        <v>4.39200496673584</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.2832817435264587</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>logs/results_129.log</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>weights/model_129.ckpt</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>tb/129/non_robust</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>(6.1136856, 5.94682, 5.023512)</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>(89.689964, 6.5303106, 6.9162097, 5.481721)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>10</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1144559d8&gt;</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0.9943240284919739</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.5051599740982056</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.03973168134689331</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.01183739490807056</v>
+      </c>
+      <c r="K35" t="n">
+        <v>2.244748830795288</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.5051599740982056</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>logs/results_130.log</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>weights/model_130.ckpt</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>tb/130/non_robust</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>(5.440068, 6.6267796, 4.2711906)</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>(82.41523, 6.8290577, 6.507764, 4.9411907)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>10</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10d4c29d8&gt;</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>0.9939898252487183</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.9805825352668762</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.6028664112091064</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.01009145844727755</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.03882191702723503</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.9805825352668762</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>logs/results_131.log</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>weights/model_131.ckpt</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>tb/131/non_robust</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>(6.3093457, 3.5070229, 1.0974236)</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>(112.37304, 6.8774586, 7.509019, 4.2186747)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>10</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x128d489d8&gt;</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0.9889042973518372</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.9634766578674316</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.598705530166626</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.01923604309558868</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.07339794933795929</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.9634766578674316</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>logs/results_132.log</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>weights/model_132.ckpt</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>tb/132/non_robust</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>(4.4108233, 4.0895247, 2.098783)</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>(121.883095, 7.579876, 7.0298843, 4.9557033)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>10</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10cb379d8&gt;</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0.9932920336723328</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.4969040155410767</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.05521155893802643</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.01835296675562859</v>
+      </c>
+      <c r="K38" t="n">
+        <v>2.554305791854858</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.4969040155410767</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>logs/results_133.log</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>weights/model_133.ckpt</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>tb/133/non_robust</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>(5.3379345, 6.590775, 7.8176637)</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>(85.53205, 6.9328337, 6.700486, 4.8025503)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>10</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10b8f09d8&gt;</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0.9948400259017944</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.4489164054393768</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.03044375590980053</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.009667842648923397</v>
+      </c>
+      <c r="K39" t="n">
+        <v>2.220386981964111</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.4489164054393768</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>logs/results_134.log</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>weights/model_134.ckpt</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>tb/134/non_robust</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>(5.831529, 5.42288, 4.6121693)</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>(84.4739, 6.493887, 6.5718474, 4.5377927)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>10</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x126b069d8&gt;</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0.9927760362625122</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.396284818649292</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.1434468477964401</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.0217659305781126</v>
+      </c>
+      <c r="K40" t="n">
+        <v>3.844486474990845</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.396284818649292</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>logs/results_135.log</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>weights/model_135.ckpt</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>tb/135/non_robust</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>(5.574842, 6.245333, 4.810837)</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>(85.19683, 6.5148034, 5.9850945, 4.801436)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>10</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10c6839d8&gt;</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0.9938080310821533</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.3436532616615295</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.05417956784367561</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.01406121347099543</v>
+      </c>
+      <c r="K41" t="n">
+        <v>3.211456298828125</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.3436532616615295</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>logs/results_136.log</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>weights/model_136.ckpt</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>tb/136/non_robust</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>(5.6092257, 4.143113, 3.8079915)</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>(86.52191, 5.964658, 6.166412, 5.197654)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>10</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10c0739d8&gt;</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0.9969040155410767</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.4840041399002075</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.3957688212394714</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.005571624264121056</v>
+      </c>
+      <c r="K42" t="n">
+        <v>2.366345643997192</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.4840041399002075</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>logs/results_137.log</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>weights/model_137.ckpt</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>tb/137/non_robust</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>(5.181602, 5.7295084, 5.6048174)</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>(82.88454, 7.249249, 6.479921, 3.6827447)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>10</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x122bf09d8&gt;</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>0.9922600388526917</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.3849329352378845</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.08410732448101044</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.01534473709762096</v>
+      </c>
+      <c r="K43" t="n">
+        <v>3.297931432723999</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.3849329352378845</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>logs/results_138.log</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>weights/model_138.ckpt</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>tb/138/non_robust</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>(6.15226, 7.3465576, 6.434499)</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>(82.45929, 6.825841, 6.791462, 4.857772)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>10</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1085149d8&gt;</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>0.9901960492134094</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.4520123898983002</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.01481962483376265</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1.854000926017761</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.4520123898983002</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>logs/results_139.log</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>weights/model_139.ckpt</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>tb/139/non_robust</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>(6.1308837, 4.6139526, 3.4184794)</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>(79.28881, 6.3374586, 6.397517, 4.7318683)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>10</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1236079d8&gt;</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0.9938080310821533</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.4458204209804535</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.02941176481544971</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.01214468479156494</v>
+      </c>
+      <c r="K45" t="n">
+        <v>2.593406200408936</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0.4458204209804535</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>logs/results_140.log</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>weights/model_140.ckpt</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>tb/140/non_robust</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>(5.9793363, 4.7563915, 3.7439911)</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>(83.531364, 5.821826, 6.3146667, 6.247338)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>10</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10b80c9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>0.9542302489280701</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.2746185958385468</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.9292649030685425</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.273960679769516</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1.318848848342896</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0.2746185958385468</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>logs/results_144.log</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>weights/model_144.ckpt</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>tb/144/non_robust</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>(1.3802013, 1.1343896, 0.76373345)</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>(34.742443, 5.622468, 5.3874836, 6.303792)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>100</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10ee679d8&gt;</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>0.9907535910606384</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.3273231685161591</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.9879796504974365</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.02232153527438641</v>
+      </c>
+      <c r="K47" t="n">
+        <v>1.997956991195679</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.3273231685161591</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>logs/results_145.log</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>weights/model_145.ckpt</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>tb/145/non_robust</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>(1.7613791, 2.3774006, 2.0184257)</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>(32.95792, 5.2022047, 5.127589, 4.6593046)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Singular values notebook p good and pgd adv train works with ugly graph copies
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1504,6 +1504,207 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>30</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1104e69d8&gt;</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>0.8981999754905701</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.3424000144004822</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.04809999838471413</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.3424164950847626</v>
+      </c>
+      <c r="K19" t="n">
+        <v>3.330149173736572</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.3424000144004822</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>logs/results_121.log</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>weights/model_121.ckpt</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>tb/121/non_robust</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>(1.4056362, 3.0716696, 6.664684, 11.19474, 13.153981, 10.241105, 6.051113)</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>(24.022184, 14.81685, 21.985281, 18.528912, 16.116236, 15.134631, 11.263296, 22.44767)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>30</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10df1b9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9559000134468079</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.2694000005722046</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.05429999902844429</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.1658958792686462</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4.698654651641846</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.2694000005722046</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>logs/results_123.log</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>weights/model_123.ckpt</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>tb/123/non_robust</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>(0.3431952, 0.41664022, 0.5683927, 0.91492766, 1.3893795, 2.3776739, 3.8029735)</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>(6.3056436, 7.597117, 7.726599, 8.445029, 7.708117, 7.5270963, 7.9869733, 9.796146)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>30</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x119b5f9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>0.8652999997138977</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.1185000017285347</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.005900000222027302</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.4752624034881592</v>
+      </c>
+      <c r="K21" t="n">
+        <v>3.402863264083862</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.1185000017285347</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>logs/results_126.log</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>weights/model_126.ckpt</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>tb/126/non_robust</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>(0.90816385, 0.7060737, 0.9453165, 1.4311132, 1.8074349, 2.626249, 3.3506863)</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>(15.063638, 2.4488645, 2.8450708, 3.4224455, 2.870352, 2.775072, 2.7803397, 3.6928034)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Now the PGD values get properly clipped
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,6 +1705,207 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11c4be9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>0.9559000134468079</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.05790000036358833</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.04890000075101852</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.1738029420375824</v>
+      </c>
+      <c r="K22" t="n">
+        <v>6.665348529815674</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.05790000036358833</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>logs/results_222.log</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>weights/model_222.ckpt</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>tb/222/non_robust</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>(7.230026, 8.443772, 9.982576, 10.426454, 10.48337, 10.4655, 8.748777)</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>(139.92761, 9.773078, 8.607171, 8.341426, 7.4237742, 7.5570107, 6.5512905, 8.353663)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11e21a9d8&gt;</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>0.9312000274658203</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.06909999996423721</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.1206000000238419</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.2596416771411896</v>
+      </c>
+      <c r="K23" t="n">
+        <v>7.456814289093018</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.06909999996423721</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>logs/results_232.log</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>weights/model_232.ckpt</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>tb/232/non_robust</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>(7.3609123, 7.8955326, 9.737668, 9.91078, 10.763038, 10.914308, 9.4478855)</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>(140.87561, 8.819877, 8.838883, 8.998733, 7.921186, 7.691656, 7.321085, 9.176294)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x111a129d8&gt;</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>0.9312999844551086</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.03830000013113022</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.009100000374019146</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.2439231872558594</v>
+      </c>
+      <c r="K24" t="n">
+        <v>7.289804458618164</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.03830000013113022</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>logs/results_234.log</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>weights/model_234.ckpt</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>tb/234/non_robust</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>(7.0172796, 7.6613173, 8.302304, 8.662146, 7.9462867, 9.3396435, 7.44935)</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>(136.32106, 9.159889, 8.33736, 8.452992, 7.9244547, 7.2932935, 7.7801814, 9.626968)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added early stopping and new script for hyperparam search
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -389,65 +389,80 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>adv_train_flag</t>
+          <t>training_type</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>pgd_train_eps</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>pgd_train_eta</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>pgd_train_num_iter</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>activation</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>acc_reg</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>acc_fgsm</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>acc_pgd</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>loss_reg</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>loss_pgd</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>loss_fgsm</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>logdir</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>weights_path</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>tb_dir</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Distances</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Norms</t>
         </is>
@@ -471,34 +486,37 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
         <is>
           <t>Sigmoid</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="J2" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="H2" t="n">
+      <c r="K2" t="n">
         <v>67.59999999999999</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
         <v>0.2</v>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="n">
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="n">
         <v>0.8</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr">
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
@@ -522,42 +540,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>0.7243999838829041</v>
       </c>
-      <c r="H3" t="n">
+      <c r="K3" t="n">
         <v>0.05319999903440475</v>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
         <v>0.8155719041824341</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="n">
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="n">
         <v>5.454379558563232</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>logs/results_11.log</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
         <is>
           <t>tb/11/non_robust</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
@@ -581,42 +602,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>0.7918999791145325</v>
       </c>
-      <c r="H4" t="n">
+      <c r="K4" t="n">
         <v>0.05810000002384186</v>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
         <v>0.6927952170372009</v>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="n">
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
         <v>4.691385269165039</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>logs/results_13.log</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
         <is>
           <t>tb/13/non_robust</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>(0.9306673, 0.6533018, 0.6531849, 0.6674277, 0.6947321, 0.75724566, 0.7961144)</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>(&lt;tf.Tensor 'model_non_robust/Max_8:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_9:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_10:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_11:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_12:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_13:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_14:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_15:0' shape=() dtype=float32&gt;)</t>
         </is>
@@ -640,42 +664,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="J5" t="n">
         <v>0.9466999769210815</v>
       </c>
-      <c r="H5" t="n">
+      <c r="K5" t="n">
         <v>0.1215000003576279</v>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="n">
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
         <v>0.2134527862071991</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
         <v>6.628881454467773</v>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>logs/results_41.log</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
         <is>
           <t>tb/41/non_robust</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>(0.9239762, 0.65693253, 0.6067492, 0.6374461, 0.64722586, 0.750713, 0.7882854)</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>(319.44058, 36.396854, 20.660694, 23.362183, 24.99871, 29.359327, 33.84145, 27.05041)</t>
         </is>
@@ -699,42 +726,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="J6" t="n">
         <v>0.9369000196456909</v>
       </c>
-      <c r="H6" t="n">
+      <c r="K6" t="n">
         <v>0.1234000027179718</v>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
         <v>0.2546896040439606</v>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="n">
         <v>6.354927062988281</v>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>logs/results_42.log</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
         <is>
           <t>tb/42/non_robust</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>(0.9097431, 0.59459233, 0.6237213, 0.646627, 0.70321494, 0.7542059, 0.80426776)</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>(325.33728, 32.12922, 22.591274, 19.652607, 20.43904, 26.104446, 38.55416, 27.83214)</t>
         </is>
@@ -758,42 +788,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="J7" t="n">
         <v>0.9275000095367432</v>
       </c>
-      <c r="H7" t="n">
+      <c r="K7" t="n">
         <v>0.0681999996304512</v>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="n">
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
         <v>0.297708123922348</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="n">
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="n">
         <v>7.019247531890869</v>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>logs/results_43.log</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr">
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
         <is>
           <t>tb/43/non_robust</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>(0.8931245, 0.56005055, 0.59760016, 0.57427925, 0.6759137, 0.76545215, 0.78780127)</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>(326.3446, 31.664152, 22.359634, 21.57176, 27.57798, 34.183285, 35.271046, 29.007282)</t>
         </is>
@@ -817,42 +850,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="J8" t="n">
         <v>0.944100022315979</v>
       </c>
-      <c r="H8" t="n">
+      <c r="K8" t="n">
         <v>0.01999999955296516</v>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
         <v>0.246184840798378</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="n">
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
         <v>8.873349189758301</v>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>logs/results_44.log</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr">
         <is>
           <t>tb/44/non_robust</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>(0.938725, 0.6600768, 0.66170657, 0.6852295, 0.7025278, 0.7467286, 0.76420873)</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>(329.55527, 26.631884, 20.483023, 21.433125, 23.539381, 28.294022, 27.846375, 27.025381)</t>
         </is>
@@ -876,42 +912,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="J9" t="n">
         <v>0.9415000081062317</v>
       </c>
-      <c r="H9" t="n">
+      <c r="K9" t="n">
         <v>0.2319000065326691</v>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="n">
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
         <v>0.2557807564735413</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="n">
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="n">
         <v>5.129439353942871</v>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>logs/results_45.log</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
         <is>
           <t>tb/45/non_robust</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>(0.92154706, 0.6415282, 0.6576658, 0.6670158, 0.700283, 0.7661101, 0.80726135)</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>(332.50662, 27.713497, 22.988976, 24.210987, 22.345839, 28.06629, 34.470566, 28.11802)</t>
         </is>
@@ -935,42 +974,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
         <is>
           <t>Relu</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="J10" t="n">
         <v>0.9623000025749207</v>
       </c>
-      <c r="H10" t="n">
+      <c r="K10" t="n">
         <v>0.03970000147819519</v>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
         <v>0.1634003221988678</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="n">
         <v>8.993168830871582</v>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>logs/results_46.log</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr">
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
         <is>
           <t>tb/46/non_robust</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>(13.717814, 18.26012, 24.893442, 31.145538, 29.057154, 20.91586, 15.984089)</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>(267.34714, 12.150078, 13.141031, 13.2189455, 9.97285, 8.843685, 8.705187, 13.771522)</t>
         </is>
@@ -994,42 +1036,45 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
         <is>
           <t>Relu</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="J11" t="n">
         <v>0.9621999859809875</v>
       </c>
-      <c r="H11" t="n">
+      <c r="K11" t="n">
         <v>0.06289999932050705</v>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="n">
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
         <v>0.1620544195175171</v>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="n">
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="n">
         <v>28.44748115539551</v>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>logs/results_47.log</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
         <is>
           <t>tb/47/non_robust</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>(13.70231, 18.81006, 24.938885, 29.81304, 33.936825, 19.185276, 17.508503)</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>(281.3783, 12.946939, 12.665519, 12.067004, 9.140996, 9.732248, 8.472949, 14.707483)</t>
         </is>
@@ -1053,50 +1098,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
         <is>
           <t>Relu</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="J12" t="n">
         <v>0.9298999905586243</v>
       </c>
-      <c r="H12" t="n">
+      <c r="K12" t="n">
         <v>0.03920000046491623</v>
       </c>
-      <c r="I12" t="n">
+      <c r="L12" t="n">
         <v>0.006000000052154064</v>
       </c>
-      <c r="J12" t="n">
+      <c r="M12" t="n">
         <v>0.2370504885911942</v>
       </c>
-      <c r="K12" t="n">
+      <c r="N12" t="n">
         <v>6.775509357452393</v>
       </c>
-      <c r="L12" t="n">
+      <c r="O12" t="n">
         <v>0.03920000046491623</v>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>logs/results_57.log</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>weights/model_57.ckpt</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>tb/57/non_robust</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>(7.4477954, 6.8025093, 7.2666335, 7.3556733, 8.691928, 8.399956, 8.053249)</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>(138.91463, 9.132495, 8.988977, 8.27085, 8.298483, 7.1643567, 7.5375657, 11.348869)</t>
         </is>
@@ -1120,50 +1168,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x117e589d8&gt;</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="J13" t="n">
         <v>0.9531000256538391</v>
       </c>
-      <c r="H13" t="n">
+      <c r="K13" t="n">
         <v>0.04850000143051147</v>
       </c>
-      <c r="I13" t="n">
+      <c r="L13" t="n">
         <v>0.01339999958872795</v>
       </c>
-      <c r="J13" t="n">
+      <c r="M13" t="n">
         <v>0.1710376739501953</v>
       </c>
-      <c r="K13" t="n">
+      <c r="N13" t="n">
         <v>6.398704528808594</v>
       </c>
-      <c r="L13" t="n">
+      <c r="O13" t="n">
         <v>0.04850000143051147</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>logs/results_58.log</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>weights/model_58.ckpt</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="R13" t="inlineStr">
         <is>
           <t>tb/58/non_robust</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>(7.135254, 7.887454, 7.845998, 8.052931, 8.5888, 8.207241, 6.9763064)</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>(140.55019, 9.100359, 9.088696, 8.028114, 8.66318, 7.551326, 7.209709, 10.0992565)</t>
         </is>
@@ -1187,50 +1238,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11ad159d8&gt;</t>
         </is>
       </c>
-      <c r="G14" t="n">
+      <c r="J14" t="n">
         <v>0.9657999873161316</v>
       </c>
-      <c r="H14" t="n">
+      <c r="K14" t="n">
         <v>0.2011000066995621</v>
       </c>
-      <c r="I14" t="n">
+      <c r="L14" t="n">
         <v>0.1811999976634979</v>
       </c>
-      <c r="J14" t="n">
+      <c r="M14" t="n">
         <v>0.1451183259487152</v>
       </c>
-      <c r="K14" t="n">
+      <c r="N14" t="n">
         <v>5.327450752258301</v>
       </c>
-      <c r="L14" t="n">
+      <c r="O14" t="n">
         <v>0.2011000066995621</v>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>logs/results_71.log</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>weights/model_71.ckpt</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>tb/71/non_robust</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>(5.475276, 12.719564, 18.869154, 27.198263, 26.215324, 22.13533, 16.86695)</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>(78.487724, 11.971958, 8.304008, 4.5321946, 2.381914, 1.7097418, 1.7520251, 2.2926486)</t>
         </is>
@@ -1254,50 +1308,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x12008f9d8&gt;</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="J15" t="n">
         <v>0.9585999846458435</v>
       </c>
-      <c r="H15" t="n">
+      <c r="K15" t="n">
         <v>0.2369000017642975</v>
       </c>
-      <c r="I15" t="n">
+      <c r="L15" t="n">
         <v>0.03700000047683716</v>
       </c>
-      <c r="J15" t="n">
+      <c r="M15" t="n">
         <v>0.1429557055234909</v>
       </c>
-      <c r="K15" t="n">
+      <c r="N15" t="n">
         <v>4.122503280639648</v>
       </c>
-      <c r="L15" t="n">
+      <c r="O15" t="n">
         <v>0.2369000017642975</v>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>logs/results_72.log</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>weights/model_72.ckpt</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>tb/72/non_robust</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="S15" t="inlineStr">
         <is>
           <t>(2.139943, 3.496155, 3.843952, 5.1138744, 6.2203045, 6.9547405, 8.452685)</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>(29.190838, 5.508862, 3.9576876, 1.9097207, 1.488211, 1.3313731, 1.552425, 1.4604229)</t>
         </is>
@@ -1321,50 +1378,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1240199d8&gt;</t>
         </is>
       </c>
-      <c r="G16" t="n">
+      <c r="J16" t="n">
         <v>0.9384999871253967</v>
       </c>
-      <c r="H16" t="n">
+      <c r="K16" t="n">
         <v>0.2345000058412552</v>
       </c>
-      <c r="I16" t="n">
+      <c r="L16" t="n">
         <v>0.07829999923706055</v>
       </c>
-      <c r="J16" t="n">
+      <c r="M16" t="n">
         <v>0.2154168486595154</v>
       </c>
-      <c r="K16" t="n">
+      <c r="N16" t="n">
         <v>4.516582012176514</v>
       </c>
-      <c r="L16" t="n">
+      <c r="O16" t="n">
         <v>0.2345000058412552</v>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>logs/results_74.log</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>weights/model_74.ckpt</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>tb/74/non_robust</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>(1.7076006, 2.5921235, 2.5732467, 3.4120953, 4.31576, 5.6463065, 6.7571893)</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>(23.436884, 4.6997, 2.8007762, 1.6223694, 1.4685857, 1.5694603, 1.4128212, 1.4283097)</t>
         </is>
@@ -1388,50 +1448,53 @@
           <t>FGSM</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11951f9d8&gt;</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="J17" t="n">
         <v>0.9517999887466431</v>
       </c>
-      <c r="H17" t="n">
+      <c r="K17" t="n">
         <v>0.8098999857902527</v>
       </c>
-      <c r="I17" t="n">
+      <c r="L17" t="n">
         <v>0.4519999921321869</v>
       </c>
-      <c r="J17" t="n">
+      <c r="M17" t="n">
         <v>0.1830078810453415</v>
       </c>
-      <c r="K17" t="n">
+      <c r="N17" t="n">
         <v>0.6702156066894531</v>
       </c>
-      <c r="L17" t="n">
+      <c r="O17" t="n">
         <v>0.8098999857902527</v>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>logs/results_75.log</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>weights/model_75.ckpt</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="R17" t="inlineStr">
         <is>
           <t>tb/75/robust</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="S17" t="inlineStr">
         <is>
           <t>(6.767173, 17.473831, 38.257633, 49.1879, 27.285254, 10.4143715, 4.247443)</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="T17" t="inlineStr">
         <is>
           <t>(131.64798, 17.081043, 17.57381, 15.574147, 13.246862, 13.433027, 11.568809, 11.362484)</t>
         </is>
@@ -1455,50 +1518,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x122d779d8&gt;</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="J18" t="n">
         <v>0.4650999903678894</v>
       </c>
-      <c r="H18" t="n">
+      <c r="K18" t="n">
         <v>0.1655000001192093</v>
       </c>
-      <c r="I18" t="n">
+      <c r="L18" t="n">
         <v>0.1686999946832657</v>
       </c>
-      <c r="J18" t="n">
+      <c r="M18" t="n">
         <v>1.41247832775116</v>
       </c>
-      <c r="K18" t="n">
+      <c r="N18" t="n">
         <v>9.054192543029785</v>
       </c>
-      <c r="L18" t="n">
+      <c r="O18" t="n">
         <v>0.1655000001192093</v>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>logs/results_114.log</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>weights/model_114.ckpt</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="R18" t="inlineStr">
         <is>
           <t>tb/114/non_robust</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="S18" t="inlineStr">
         <is>
           <t>(12.642895, 17.784021, 41.321377, 30.120796, 45.800076, 61.19117, 119.545975)</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="T18" t="inlineStr">
         <is>
           <t>(541.2144, 24.83513, 24.277227, 26.669617, 24.392954, 26.32083, 27.765806, 23.421999)</t>
         </is>
@@ -1522,50 +1588,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1104e69d8&gt;</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="J19" t="n">
         <v>0.8981999754905701</v>
       </c>
-      <c r="H19" t="n">
+      <c r="K19" t="n">
         <v>0.3424000144004822</v>
       </c>
-      <c r="I19" t="n">
+      <c r="L19" t="n">
         <v>0.04809999838471413</v>
       </c>
-      <c r="J19" t="n">
+      <c r="M19" t="n">
         <v>0.3424164950847626</v>
       </c>
-      <c r="K19" t="n">
+      <c r="N19" t="n">
         <v>3.330149173736572</v>
       </c>
-      <c r="L19" t="n">
+      <c r="O19" t="n">
         <v>0.3424000144004822</v>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>logs/results_121.log</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="Q19" t="inlineStr">
         <is>
           <t>weights/model_121.ckpt</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="R19" t="inlineStr">
         <is>
           <t>tb/121/non_robust</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="S19" t="inlineStr">
         <is>
           <t>(1.4056362, 3.0716696, 6.664684, 11.19474, 13.153981, 10.241105, 6.051113)</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="T19" t="inlineStr">
         <is>
           <t>(24.022184, 14.81685, 21.985281, 18.528912, 16.116236, 15.134631, 11.263296, 22.44767)</t>
         </is>
@@ -1589,50 +1658,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x10df1b9d8&gt;</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="J20" t="n">
         <v>0.9559000134468079</v>
       </c>
-      <c r="H20" t="n">
+      <c r="K20" t="n">
         <v>0.2694000005722046</v>
       </c>
-      <c r="I20" t="n">
+      <c r="L20" t="n">
         <v>0.05429999902844429</v>
       </c>
-      <c r="J20" t="n">
+      <c r="M20" t="n">
         <v>0.1658958792686462</v>
       </c>
-      <c r="K20" t="n">
+      <c r="N20" t="n">
         <v>4.698654651641846</v>
       </c>
-      <c r="L20" t="n">
+      <c r="O20" t="n">
         <v>0.2694000005722046</v>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>logs/results_123.log</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
         <is>
           <t>weights/model_123.ckpt</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="R20" t="inlineStr">
         <is>
           <t>tb/123/non_robust</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
+      <c r="S20" t="inlineStr">
         <is>
           <t>(0.3431952, 0.41664022, 0.5683927, 0.91492766, 1.3893795, 2.3776739, 3.8029735)</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="T20" t="inlineStr">
         <is>
           <t>(6.3056436, 7.597117, 7.726599, 8.445029, 7.708117, 7.5270963, 7.9869733, 9.796146)</t>
         </is>
@@ -1656,50 +1728,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x119b5f9d8&gt;</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="J21" t="n">
         <v>0.8652999997138977</v>
       </c>
-      <c r="H21" t="n">
+      <c r="K21" t="n">
         <v>0.1185000017285347</v>
       </c>
-      <c r="I21" t="n">
+      <c r="L21" t="n">
         <v>0.005900000222027302</v>
       </c>
-      <c r="J21" t="n">
+      <c r="M21" t="n">
         <v>0.4752624034881592</v>
       </c>
-      <c r="K21" t="n">
+      <c r="N21" t="n">
         <v>3.402863264083862</v>
       </c>
-      <c r="L21" t="n">
+      <c r="O21" t="n">
         <v>0.1185000017285347</v>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>logs/results_126.log</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>weights/model_126.ckpt</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr">
+      <c r="R21" t="inlineStr">
         <is>
           <t>tb/126/non_robust</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="S21" t="inlineStr">
         <is>
           <t>(0.90816385, 0.7060737, 0.9453165, 1.4311132, 1.8074349, 2.626249, 3.3506863)</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="T21" t="inlineStr">
         <is>
           <t>(15.063638, 2.4488645, 2.8450708, 3.4224455, 2.870352, 2.775072, 2.7803397, 3.6928034)</t>
         </is>
@@ -1723,50 +1798,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11c4be9d8&gt;</t>
         </is>
       </c>
-      <c r="G22" t="n">
+      <c r="J22" t="n">
         <v>0.9559000134468079</v>
       </c>
-      <c r="H22" t="n">
+      <c r="K22" t="n">
         <v>0.05790000036358833</v>
       </c>
-      <c r="I22" t="n">
+      <c r="L22" t="n">
         <v>0.04890000075101852</v>
       </c>
-      <c r="J22" t="n">
+      <c r="M22" t="n">
         <v>0.1738029420375824</v>
       </c>
-      <c r="K22" t="n">
+      <c r="N22" t="n">
         <v>6.665348529815674</v>
       </c>
-      <c r="L22" t="n">
+      <c r="O22" t="n">
         <v>0.05790000036358833</v>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="P22" t="inlineStr">
         <is>
           <t>logs/results_222.log</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr">
+      <c r="Q22" t="inlineStr">
         <is>
           <t>weights/model_222.ckpt</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="R22" t="inlineStr">
         <is>
           <t>tb/222/non_robust</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
+      <c r="S22" t="inlineStr">
         <is>
           <t>(7.230026, 8.443772, 9.982576, 10.426454, 10.48337, 10.4655, 8.748777)</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="T22" t="inlineStr">
         <is>
           <t>(139.92761, 9.773078, 8.607171, 8.341426, 7.4237742, 7.5570107, 6.5512905, 8.353663)</t>
         </is>
@@ -1790,50 +1868,53 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11e21a9d8&gt;</t>
         </is>
       </c>
-      <c r="G23" t="n">
+      <c r="J23" t="n">
         <v>0.9312000274658203</v>
       </c>
-      <c r="H23" t="n">
+      <c r="K23" t="n">
         <v>0.06909999996423721</v>
       </c>
-      <c r="I23" t="n">
+      <c r="L23" t="n">
         <v>0.1206000000238419</v>
       </c>
-      <c r="J23" t="n">
+      <c r="M23" t="n">
         <v>0.2596416771411896</v>
       </c>
-      <c r="K23" t="n">
+      <c r="N23" t="n">
         <v>7.456814289093018</v>
       </c>
-      <c r="L23" t="n">
+      <c r="O23" t="n">
         <v>0.06909999996423721</v>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="P23" t="inlineStr">
         <is>
           <t>logs/results_232.log</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr">
+      <c r="Q23" t="inlineStr">
         <is>
           <t>weights/model_232.ckpt</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
+      <c r="R23" t="inlineStr">
         <is>
           <t>tb/232/non_robust</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
+      <c r="S23" t="inlineStr">
         <is>
           <t>(7.3609123, 7.8955326, 9.737668, 9.91078, 10.763038, 10.914308, 9.4478855)</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
+      <c r="T23" t="inlineStr">
         <is>
           <t>(140.87561, 8.819877, 8.838883, 8.998733, 7.921186, 7.691656, 7.321085, 9.176294)</t>
         </is>
@@ -1857,54 +1938,261 @@
           <t>Regular</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x111a129d8&gt;</t>
         </is>
       </c>
-      <c r="G24" t="n">
+      <c r="J24" t="n">
         <v>0.9312999844551086</v>
       </c>
-      <c r="H24" t="n">
+      <c r="K24" t="n">
         <v>0.03830000013113022</v>
       </c>
-      <c r="I24" t="n">
+      <c r="L24" t="n">
         <v>0.009100000374019146</v>
       </c>
-      <c r="J24" t="n">
+      <c r="M24" t="n">
         <v>0.2439231872558594</v>
       </c>
-      <c r="K24" t="n">
+      <c r="N24" t="n">
         <v>7.289804458618164</v>
       </c>
-      <c r="L24" t="n">
+      <c r="O24" t="n">
         <v>0.03830000013113022</v>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="P24" t="inlineStr">
         <is>
           <t>logs/results_234.log</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr">
+      <c r="Q24" t="inlineStr">
         <is>
           <t>weights/model_234.ckpt</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="R24" t="inlineStr">
         <is>
           <t>tb/234/non_robust</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr">
+      <c r="S24" t="inlineStr">
         <is>
           <t>(7.0172796, 7.6613173, 8.302304, 8.662146, 7.9462867, 9.3396435, 7.44935)</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
+      <c r="T24" t="inlineStr">
         <is>
           <t>(136.32106, 9.159889, 8.33736, 8.452992, 7.9244547, 7.2932935, 7.7801814, 9.626968)</t>
         </is>
       </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>PGD</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>3</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x118b969d8&gt;</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>0.8787999749183655</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.01040000002831221</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.001300000003539026</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.4310351014137268</v>
+      </c>
+      <c r="N25" t="n">
+        <v>8.296195983886719</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.01040000002831221</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>logs/results_278.log</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>weights/model_278.ckpt</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>tb/278/robust</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>PGD</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x121b0f9d8&gt;</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>0.8522999882698059</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.002899999963119626</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.5192863941192627</v>
+      </c>
+      <c r="N26" t="n">
+        <v>9.538139343261719</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.002899999963119626</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>logs/results_279.log</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>weights/model_279.ckpt</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>tb/279/robust</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>PGD</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x121b0f9d8&gt;</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>0.8676999807357788</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.004999999888241291</v>
+      </c>
+      <c r="L27" t="n">
+        <v>9.999999747378752e-05</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.4790646433830261</v>
+      </c>
+      <c r="N27" t="n">
+        <v>9.238405227661133</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.004999999888241291</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>logs/results_279.log</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>weights/model_279.ckpt</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>tb/279/robust</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Wrote code to find margin proxy by attacking in featurization space - untested
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2194,6 +2194,216 @@
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
     </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10f4d69d8&gt;</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>0.9516000151634216</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.04560000076889992</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.003700000001117587</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.1825118958950043</v>
+      </c>
+      <c r="N28" t="n">
+        <v>6.906796932220459</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.04560000076889992</v>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>logs/results_282.log</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>weights/model_282.ckpt</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>tb/282</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>(6.9546156, 7.3834124, 9.092276, 9.433221, 9.5498905, 11.14911, 9.904368)</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>(139.42224, 9.018682, 9.271418, 8.975029, 7.9992733, 7.393931, 7.053868, 10.015819)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1100289d8&gt;</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>0.9430999755859375</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.06279999762773514</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.006200000178068876</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.2192680686712265</v>
+      </c>
+      <c r="N29" t="n">
+        <v>7.151318073272705</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.06279999762773514</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>logs/results_285.log</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>weights/model_285.ckpt</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>tb/285</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>(7.0936155, 7.6124697, 8.267413, 8.219525, 11.057663, 10.19839, 9.6345)</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>(141.34113, 8.731318, 9.105043, 8.344593, 9.322138, 7.830576, 7.469233, 9.507704)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x116aa89d8&gt;</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>0.9474999904632568</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.07349999994039536</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.03050000034272671</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.2007102072238922</v>
+      </c>
+      <c r="N30" t="n">
+        <v>6.25114631652832</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.07349999994039536</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>logs/results_305.log</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>weights/model_305.ckpt</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>tb/305</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>(6.9461164, 7.606389, 7.896417, 8.789286, 9.165759, 8.689637, 8.321884)</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>(138.02159, 8.655811, 9.216804, 9.208384, 7.499287, 7.888038, 7.191258, 13.024145)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added bug report file
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2404,6 +2404,566 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>FGSM</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x128d789d8&gt;</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>0.9329000115394592</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.7416999936103821</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.5971999764442444</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.2206476628780365</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.74456787109375</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.7416999936103821</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>logs/results_328.log</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>weights/model_328.ckpt</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>tb/328</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>(12.799518, 16.56418, 25.464622, 25.766693, 14.9766655, 6.904501, 3.7851212)</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>(309.03058, 13.829748, 16.421766, 12.924315, 13.326067, 11.006118, 10.691159, 13.276878)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x113fe39d8&gt;</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>0.9472000002861023</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.3325000107288361</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.1923000067472458</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.1799724549055099</v>
+      </c>
+      <c r="N32" t="n">
+        <v>3.20237398147583</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.3325000107288361</v>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>logs/results_331.log</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>weights/model_331.ckpt</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>tb/331</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>(1.8040013, 1.8094578, 1.9554862, 2.5528448, 3.399231, 4.635884, 6.39143)</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>(28.089184, 4.674623, 3.6114936, 3.2815678, 3.1776936, 2.116904, 2.2179012, 2.6026235)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x118f1b9d8&gt;</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>0.8956000208854675</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.3217999935150146</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.2044000029563904</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.3738516569137573</v>
+      </c>
+      <c r="N33" t="n">
+        <v>3.476548433303833</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.3217999935150146</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>logs/results_332.log</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>weights/model_332.ckpt</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>tb/332</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>(1.4544966, 1.1530415, 1.2943891, 2.1282125, 4.040144, 7.1142826, 6.1251535)</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>(21.872171, 4.500764, 3.899859, 2.0486226, 2.4281611, 2.2534535, 1.7587844, 2.4474022)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>60</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x10b0f09d8&gt;</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>0.9347000122070312</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.2572999894618988</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.1509999930858612</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.2364677786827087</v>
+      </c>
+      <c r="N34" t="n">
+        <v>4.247204780578613</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.2572999894618988</v>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>logs/results_333.log</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>weights/model_333.ckpt</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>tb/333</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>(0.4250503, 0.4371529, 0.74407357, 1.2906153, 2.5302472, 4.9194384, 6.6656017)</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>(6.92537, 5.7589846, 3.67073, 3.039194, 3.1920185, 5.1396704, 3.4247825, 4.5205474)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>60</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1.5e-05</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1113b09d8&gt;</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>0.9394999742507935</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.09109999984502792</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.03319999948143959</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.221238300204277</v>
+      </c>
+      <c r="N35" t="n">
+        <v>6.377280712127686</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.09109999984502792</v>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>logs/results_336.log</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>weights/model_336.ckpt</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>tb/336</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>(2.0724185, 1.3095005, 1.6185311, 1.3509899, 1.5398465, 1.9591715, 4.275175)</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>(39.100674, 3.319005, 3.0519383, 1.6382135, 2.70516, 2.7627785, 5.8854613, 6.491546)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>30</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2.3e-05</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1132949d8&gt;</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>0.9189000129699707</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.05869999900460243</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.02209999971091747</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.3333184719085693</v>
+      </c>
+      <c r="N36" t="n">
+        <v>6.367059707641602</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.05869999900460243</v>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>logs/results_346.log</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>weights/model_346.ckpt</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>tb/346</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>(1.5257524, 0.7150309, 0.56886697, 0.49205807, 0.57274866, 1.5198021, 4.5895967)</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>(33.718807, 2.9477801, 2.0959005, 1.7632871, 2.2024982, 4.748903, 8.546004, 6.910356)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>100</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1226c79d8&gt;</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>0.9646999835968018</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.1290999948978424</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.01889999955892563</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.1261469274759293</v>
+      </c>
+      <c r="N37" t="n">
+        <v>6.858481407165527</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.1290999948978424</v>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>logs/results_353.log</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>weights/model_353.ckpt</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>tb/353</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>(0.6469947, 0.73037505, 0.9719021, 1.3849623, 2.158197, 3.6967816, 6.6338224)</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>(9.72191, 3.5845523, 3.115291, 2.8329852, 2.7452235, 2.6821659, 2.723758, 2.6171021)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>100</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x1226499d8&gt;</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>0.9384999871253967</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.3431999981403351</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.217399999499321</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.2118040025234222</v>
+      </c>
+      <c r="N38" t="n">
+        <v>2.253601551055908</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0.3431999981403351</v>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>logs/results_354.log</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>weights/model_354.ckpt</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>tb/354</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>(0.2376155, 0.2859654, 0.43169716, 0.67097735, 1.0554945, 1.7692584, 2.8368058)</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>(3.0683854, 1.7650508, 1.7416625, 1.7273158, 1.7367424, 1.746138, 1.7387878, 1.7745363)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Split up the util functions better and wrote code to compare many models
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,85 +384,100 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>trace_first_reg</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trace_all_reg</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>l1_reg</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>learning_rate</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>training_type</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>pgd_train_eps</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>pgd_train_eta</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>pgd_train_num_iter</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>activation</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>acc_reg</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>acc_fgsm</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>acc_pgd</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>loss_reg</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>loss_pgd</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>loss_fgsm</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>logdir</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>weights_path</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>tb_dir</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Distances</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Norms</t>
         </is>
@@ -478,45 +493,48 @@
       <c r="C2" t="n">
         <v>0.0007</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
         <is>
           <t>Sigmoid</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="M2" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>67.59999999999999</v>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="n">
         <v>0.2</v>
       </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="n">
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="n">
         <v>0.8</v>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr">
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
@@ -532,53 +550,56 @@
       <c r="C3" t="n">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
         <v>0.003</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="M3" t="n">
         <v>0.7243999838829041</v>
       </c>
-      <c r="K3" t="n">
+      <c r="N3" t="n">
         <v>0.05319999903440475</v>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
         <v>0.8155719041824341</v>
       </c>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="n">
         <v>5.454379558563232</v>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>logs/results_11.log</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
         <is>
           <t>tb/11/non_robust</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>(None, None)</t>
         </is>
@@ -594,53 +615,56 @@
       <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
         <v>0.003</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="M4" t="n">
         <v>0.7918999791145325</v>
       </c>
-      <c r="K4" t="n">
+      <c r="N4" t="n">
         <v>0.05810000002384186</v>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
         <v>0.6927952170372009</v>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="n">
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="n">
         <v>4.691385269165039</v>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>logs/results_13.log</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr">
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
         <is>
           <t>tb/13/non_robust</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>(0.9306673, 0.6533018, 0.6531849, 0.6674277, 0.6947321, 0.75724566, 0.7961144)</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>(&lt;tf.Tensor 'model_non_robust/Max_8:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_9:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_10:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_11:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_12:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_13:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_14:0' shape=() dtype=float32&gt;, &lt;tf.Tensor 'model_non_robust/Max_15:0' shape=() dtype=float32&gt;)</t>
         </is>
@@ -656,53 +680,56 @@
       <c r="C5" t="n">
         <v>0</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
         <v>0.003</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="M5" t="n">
         <v>0.9466999769210815</v>
       </c>
-      <c r="K5" t="n">
+      <c r="N5" t="n">
         <v>0.1215000003576279</v>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
         <v>0.2134527862071991</v>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="n">
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="n">
         <v>6.628881454467773</v>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>logs/results_41.log</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr">
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
         <is>
           <t>tb/41/non_robust</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>(0.9239762, 0.65693253, 0.6067492, 0.6374461, 0.64722586, 0.750713, 0.7882854)</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>(319.44058, 36.396854, 20.660694, 23.362183, 24.99871, 29.359327, 33.84145, 27.05041)</t>
         </is>
@@ -718,53 +745,56 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
         <v>0.003</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="M6" t="n">
         <v>0.9369000196456909</v>
       </c>
-      <c r="K6" t="n">
+      <c r="N6" t="n">
         <v>0.1234000027179718</v>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
         <v>0.2546896040439606</v>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="n">
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
         <v>6.354927062988281</v>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>logs/results_42.log</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr">
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
         <is>
           <t>tb/42/non_robust</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>(0.9097431, 0.59459233, 0.6237213, 0.646627, 0.70321494, 0.7542059, 0.80426776)</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="W6" t="inlineStr">
         <is>
           <t>(325.33728, 32.12922, 22.591274, 19.652607, 20.43904, 26.104446, 38.55416, 27.83214)</t>
         </is>
@@ -780,53 +810,56 @@
       <c r="C7" t="n">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
         <v>0.003</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="M7" t="n">
         <v>0.9275000095367432</v>
       </c>
-      <c r="K7" t="n">
+      <c r="N7" t="n">
         <v>0.0681999996304512</v>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
         <v>0.297708123922348</v>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="n">
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
         <v>7.019247531890869</v>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>logs/results_43.log</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr">
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
         <is>
           <t>tb/43/non_robust</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>(0.8931245, 0.56005055, 0.59760016, 0.57427925, 0.6759137, 0.76545215, 0.78780127)</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="W7" t="inlineStr">
         <is>
           <t>(326.3446, 31.664152, 22.359634, 21.57176, 27.57798, 34.183285, 35.271046, 29.007282)</t>
         </is>
@@ -842,53 +875,56 @@
       <c r="C8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
         <v>0.003</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="M8" t="n">
         <v>0.944100022315979</v>
       </c>
-      <c r="K8" t="n">
+      <c r="N8" t="n">
         <v>0.01999999955296516</v>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="n">
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
         <v>0.246184840798378</v>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="n">
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="n">
         <v>8.873349189758301</v>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>logs/results_44.log</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr">
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
         <is>
           <t>tb/44/non_robust</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="V8" t="inlineStr">
         <is>
           <t>(0.938725, 0.6600768, 0.66170657, 0.6852295, 0.7025278, 0.7467286, 0.76420873)</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="W8" t="inlineStr">
         <is>
           <t>(329.55527, 26.631884, 20.483023, 21.433125, 23.539381, 28.294022, 27.846375, 27.025381)</t>
         </is>
@@ -904,53 +940,56 @@
       <c r="C9" t="n">
         <v>0</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
         <v>0.003</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
         <is>
           <t>sigmoid</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="M9" t="n">
         <v>0.9415000081062317</v>
       </c>
-      <c r="K9" t="n">
+      <c r="N9" t="n">
         <v>0.2319000065326691</v>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="n">
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
         <v>0.2557807564735413</v>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="n">
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="n">
         <v>5.129439353942871</v>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>logs/results_45.log</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr">
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
         <is>
           <t>tb/45/non_robust</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="V9" t="inlineStr">
         <is>
           <t>(0.92154706, 0.6415282, 0.6576658, 0.6670158, 0.700283, 0.7661101, 0.80726135)</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="W9" t="inlineStr">
         <is>
           <t>(332.50662, 27.713497, 22.988976, 24.210987, 22.345839, 28.06629, 34.470566, 28.11802)</t>
         </is>
@@ -966,53 +1005,56 @@
       <c r="C10" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="n">
         <v>0.003</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
         <is>
           <t>Relu</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="M10" t="n">
         <v>0.9623000025749207</v>
       </c>
-      <c r="K10" t="n">
+      <c r="N10" t="n">
         <v>0.03970000147819519</v>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="n">
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
         <v>0.1634003221988678</v>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="n">
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="n">
         <v>8.993168830871582</v>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>logs/results_46.log</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr">
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
         <is>
           <t>tb/46/non_robust</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="V10" t="inlineStr">
         <is>
           <t>(13.717814, 18.26012, 24.893442, 31.145538, 29.057154, 20.91586, 15.984089)</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>(267.34714, 12.150078, 13.141031, 13.2189455, 9.97285, 8.843685, 8.705187, 13.771522)</t>
         </is>
@@ -1028,53 +1070,56 @@
       <c r="C11" t="n">
         <v>0</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
         <v>0.003</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr">
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
         <is>
           <t>Relu</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="M11" t="n">
         <v>0.9621999859809875</v>
       </c>
-      <c r="K11" t="n">
+      <c r="N11" t="n">
         <v>0.06289999932050705</v>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="n">
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
         <v>0.1620544195175171</v>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="n">
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="n">
         <v>28.44748115539551</v>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>logs/results_47.log</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr">
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
         <is>
           <t>tb/47/non_robust</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="V11" t="inlineStr">
         <is>
           <t>(13.70231, 18.81006, 24.938885, 29.81304, 33.936825, 19.185276, 17.508503)</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>(281.3783, 12.946939, 12.665519, 12.067004, 9.140996, 9.732248, 8.472949, 14.707483)</t>
         </is>
@@ -1090,61 +1135,64 @@
       <c r="C12" t="n">
         <v>0</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
         <v>0.003</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
         <is>
           <t>Relu</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="M12" t="n">
         <v>0.9298999905586243</v>
       </c>
-      <c r="K12" t="n">
+      <c r="N12" t="n">
         <v>0.03920000046491623</v>
       </c>
-      <c r="L12" t="n">
+      <c r="O12" t="n">
         <v>0.006000000052154064</v>
       </c>
-      <c r="M12" t="n">
+      <c r="P12" t="n">
         <v>0.2370504885911942</v>
       </c>
-      <c r="N12" t="n">
+      <c r="Q12" t="n">
         <v>6.775509357452393</v>
       </c>
-      <c r="O12" t="n">
+      <c r="R12" t="n">
         <v>0.03920000046491623</v>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>logs/results_57.log</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>weights/model_57.ckpt</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>tb/57/non_robust</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="V12" t="inlineStr">
         <is>
           <t>(7.4477954, 6.8025093, 7.2666335, 7.3556733, 8.691928, 8.399956, 8.053249)</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="W12" t="inlineStr">
         <is>
           <t>(138.91463, 9.132495, 8.988977, 8.27085, 8.298483, 7.1643567, 7.5375657, 11.348869)</t>
         </is>
@@ -1160,61 +1208,64 @@
       <c r="C13" t="n">
         <v>0</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
         <v>0.003</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x117e589d8&gt;</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="M13" t="n">
         <v>0.9531000256538391</v>
       </c>
-      <c r="K13" t="n">
+      <c r="N13" t="n">
         <v>0.04850000143051147</v>
       </c>
-      <c r="L13" t="n">
+      <c r="O13" t="n">
         <v>0.01339999958872795</v>
       </c>
-      <c r="M13" t="n">
+      <c r="P13" t="n">
         <v>0.1710376739501953</v>
       </c>
-      <c r="N13" t="n">
+      <c r="Q13" t="n">
         <v>6.398704528808594</v>
       </c>
-      <c r="O13" t="n">
+      <c r="R13" t="n">
         <v>0.04850000143051147</v>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>logs/results_58.log</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>weights/model_58.ckpt</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="U13" t="inlineStr">
         <is>
           <t>tb/58/non_robust</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="V13" t="inlineStr">
         <is>
           <t>(7.135254, 7.887454, 7.845998, 8.052931, 8.5888, 8.207241, 6.9763064)</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="W13" t="inlineStr">
         <is>
           <t>(140.55019, 9.100359, 9.088696, 8.028114, 8.66318, 7.551326, 7.209709, 10.0992565)</t>
         </is>
@@ -1230,61 +1281,64 @@
       <c r="C14" t="n">
         <v>0.001</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
         <v>0.003</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11ad159d8&gt;</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="M14" t="n">
         <v>0.9657999873161316</v>
       </c>
-      <c r="K14" t="n">
+      <c r="N14" t="n">
         <v>0.2011000066995621</v>
       </c>
-      <c r="L14" t="n">
+      <c r="O14" t="n">
         <v>0.1811999976634979</v>
       </c>
-      <c r="M14" t="n">
+      <c r="P14" t="n">
         <v>0.1451183259487152</v>
       </c>
-      <c r="N14" t="n">
+      <c r="Q14" t="n">
         <v>5.327450752258301</v>
       </c>
-      <c r="O14" t="n">
+      <c r="R14" t="n">
         <v>0.2011000066995621</v>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>logs/results_71.log</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>weights/model_71.ckpt</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="U14" t="inlineStr">
         <is>
           <t>tb/71/non_robust</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="V14" t="inlineStr">
         <is>
           <t>(5.475276, 12.719564, 18.869154, 27.198263, 26.215324, 22.13533, 16.86695)</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="W14" t="inlineStr">
         <is>
           <t>(78.487724, 11.971958, 8.304008, 4.5321946, 2.381914, 1.7097418, 1.7520251, 2.2926486)</t>
         </is>
@@ -1300,61 +1354,64 @@
       <c r="C15" t="n">
         <v>0.005</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
         <v>0.003</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x12008f9d8&gt;</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="M15" t="n">
         <v>0.9585999846458435</v>
       </c>
-      <c r="K15" t="n">
+      <c r="N15" t="n">
         <v>0.2369000017642975</v>
       </c>
-      <c r="L15" t="n">
+      <c r="O15" t="n">
         <v>0.03700000047683716</v>
       </c>
-      <c r="M15" t="n">
+      <c r="P15" t="n">
         <v>0.1429557055234909</v>
       </c>
-      <c r="N15" t="n">
+      <c r="Q15" t="n">
         <v>4.122503280639648</v>
       </c>
-      <c r="O15" t="n">
+      <c r="R15" t="n">
         <v>0.2369000017642975</v>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="S15" t="inlineStr">
         <is>
           <t>logs/results_72.log</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>weights/model_72.ckpt</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="U15" t="inlineStr">
         <is>
           <t>tb/72/non_robust</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="V15" t="inlineStr">
         <is>
           <t>(2.139943, 3.496155, 3.843952, 5.1138744, 6.2203045, 6.9547405, 8.452685)</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr">
+      <c r="W15" t="inlineStr">
         <is>
           <t>(29.190838, 5.508862, 3.9576876, 1.9097207, 1.488211, 1.3313731, 1.552425, 1.4604229)</t>
         </is>
@@ -1370,61 +1427,64 @@
       <c r="C16" t="n">
         <v>0.008</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
         <v>0.003</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1240199d8&gt;</t>
         </is>
       </c>
-      <c r="J16" t="n">
+      <c r="M16" t="n">
         <v>0.9384999871253967</v>
       </c>
-      <c r="K16" t="n">
+      <c r="N16" t="n">
         <v>0.2345000058412552</v>
       </c>
-      <c r="L16" t="n">
+      <c r="O16" t="n">
         <v>0.07829999923706055</v>
       </c>
-      <c r="M16" t="n">
+      <c r="P16" t="n">
         <v>0.2154168486595154</v>
       </c>
-      <c r="N16" t="n">
+      <c r="Q16" t="n">
         <v>4.516582012176514</v>
       </c>
-      <c r="O16" t="n">
+      <c r="R16" t="n">
         <v>0.2345000058412552</v>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>logs/results_74.log</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>weights/model_74.ckpt</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>tb/74/non_robust</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="V16" t="inlineStr">
         <is>
           <t>(1.7076006, 2.5921235, 2.5732467, 3.4120953, 4.31576, 5.6463065, 6.7571893)</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="W16" t="inlineStr">
         <is>
           <t>(23.436884, 4.6997, 2.8007762, 1.6223694, 1.4685857, 1.5694603, 1.4128212, 1.4283097)</t>
         </is>
@@ -1440,61 +1500,64 @@
       <c r="C17" t="n">
         <v>0</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
         <v>0.003</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>FGSM</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11951f9d8&gt;</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="M17" t="n">
         <v>0.9517999887466431</v>
       </c>
-      <c r="K17" t="n">
+      <c r="N17" t="n">
         <v>0.8098999857902527</v>
       </c>
-      <c r="L17" t="n">
+      <c r="O17" t="n">
         <v>0.4519999921321869</v>
       </c>
-      <c r="M17" t="n">
+      <c r="P17" t="n">
         <v>0.1830078810453415</v>
       </c>
-      <c r="N17" t="n">
+      <c r="Q17" t="n">
         <v>0.6702156066894531</v>
       </c>
-      <c r="O17" t="n">
+      <c r="R17" t="n">
         <v>0.8098999857902527</v>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="S17" t="inlineStr">
         <is>
           <t>logs/results_75.log</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="T17" t="inlineStr">
         <is>
           <t>weights/model_75.ckpt</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
+      <c r="U17" t="inlineStr">
         <is>
           <t>tb/75/robust</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
+      <c r="V17" t="inlineStr">
         <is>
           <t>(6.767173, 17.473831, 38.257633, 49.1879, 27.285254, 10.4143715, 4.247443)</t>
         </is>
       </c>
-      <c r="T17" t="inlineStr">
+      <c r="W17" t="inlineStr">
         <is>
           <t>(131.64798, 17.081043, 17.57381, 15.574147, 13.246862, 13.433027, 11.568809, 11.362484)</t>
         </is>
@@ -1510,61 +1573,64 @@
       <c r="C18" t="n">
         <v>0</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr">
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x122d779d8&gt;</t>
         </is>
       </c>
-      <c r="J18" t="n">
+      <c r="M18" t="n">
         <v>0.4650999903678894</v>
       </c>
-      <c r="K18" t="n">
+      <c r="N18" t="n">
         <v>0.1655000001192093</v>
       </c>
-      <c r="L18" t="n">
+      <c r="O18" t="n">
         <v>0.1686999946832657</v>
       </c>
-      <c r="M18" t="n">
+      <c r="P18" t="n">
         <v>1.41247832775116</v>
       </c>
-      <c r="N18" t="n">
+      <c r="Q18" t="n">
         <v>9.054192543029785</v>
       </c>
-      <c r="O18" t="n">
+      <c r="R18" t="n">
         <v>0.1655000001192093</v>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="S18" t="inlineStr">
         <is>
           <t>logs/results_114.log</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="T18" t="inlineStr">
         <is>
           <t>weights/model_114.ckpt</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr">
+      <c r="U18" t="inlineStr">
         <is>
           <t>tb/114/non_robust</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
+      <c r="V18" t="inlineStr">
         <is>
           <t>(12.642895, 17.784021, 41.321377, 30.120796, 45.800076, 61.19117, 119.545975)</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr">
+      <c r="W18" t="inlineStr">
         <is>
           <t>(541.2144, 24.83513, 24.277227, 26.669617, 24.392954, 26.32083, 27.765806, 23.421999)</t>
         </is>
@@ -1580,61 +1646,64 @@
       <c r="C19" t="n">
         <v>0.01</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
         <v>0.003</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1104e69d8&gt;</t>
         </is>
       </c>
-      <c r="J19" t="n">
+      <c r="M19" t="n">
         <v>0.8981999754905701</v>
       </c>
-      <c r="K19" t="n">
+      <c r="N19" t="n">
         <v>0.3424000144004822</v>
       </c>
-      <c r="L19" t="n">
+      <c r="O19" t="n">
         <v>0.04809999838471413</v>
       </c>
-      <c r="M19" t="n">
+      <c r="P19" t="n">
         <v>0.3424164950847626</v>
       </c>
-      <c r="N19" t="n">
+      <c r="Q19" t="n">
         <v>3.330149173736572</v>
       </c>
-      <c r="O19" t="n">
+      <c r="R19" t="n">
         <v>0.3424000144004822</v>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="S19" t="inlineStr">
         <is>
           <t>logs/results_121.log</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="T19" t="inlineStr">
         <is>
           <t>weights/model_121.ckpt</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="U19" t="inlineStr">
         <is>
           <t>tb/121/non_robust</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
+      <c r="V19" t="inlineStr">
         <is>
           <t>(1.4056362, 3.0716696, 6.664684, 11.19474, 13.153981, 10.241105, 6.051113)</t>
         </is>
       </c>
-      <c r="T19" t="inlineStr">
+      <c r="W19" t="inlineStr">
         <is>
           <t>(24.022184, 14.81685, 21.985281, 18.528912, 16.116236, 15.134631, 11.263296, 22.44767)</t>
         </is>
@@ -1650,61 +1719,64 @@
       <c r="C20" t="n">
         <v>0.02</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x10df1b9d8&gt;</t>
         </is>
       </c>
-      <c r="J20" t="n">
+      <c r="M20" t="n">
         <v>0.9559000134468079</v>
       </c>
-      <c r="K20" t="n">
+      <c r="N20" t="n">
         <v>0.2694000005722046</v>
       </c>
-      <c r="L20" t="n">
+      <c r="O20" t="n">
         <v>0.05429999902844429</v>
       </c>
-      <c r="M20" t="n">
+      <c r="P20" t="n">
         <v>0.1658958792686462</v>
       </c>
-      <c r="N20" t="n">
+      <c r="Q20" t="n">
         <v>4.698654651641846</v>
       </c>
-      <c r="O20" t="n">
+      <c r="R20" t="n">
         <v>0.2694000005722046</v>
       </c>
-      <c r="P20" t="inlineStr">
+      <c r="S20" t="inlineStr">
         <is>
           <t>logs/results_123.log</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="T20" t="inlineStr">
         <is>
           <t>weights/model_123.ckpt</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr">
+      <c r="U20" t="inlineStr">
         <is>
           <t>tb/123/non_robust</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
+      <c r="V20" t="inlineStr">
         <is>
           <t>(0.3431952, 0.41664022, 0.5683927, 0.91492766, 1.3893795, 2.3776739, 3.8029735)</t>
         </is>
       </c>
-      <c r="T20" t="inlineStr">
+      <c r="W20" t="inlineStr">
         <is>
           <t>(6.3056436, 7.597117, 7.726599, 8.445029, 7.708117, 7.5270963, 7.9869733, 9.796146)</t>
         </is>
@@ -1720,61 +1792,64 @@
       <c r="C21" t="n">
         <v>0.02</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x119b5f9d8&gt;</t>
         </is>
       </c>
-      <c r="J21" t="n">
+      <c r="M21" t="n">
         <v>0.8652999997138977</v>
       </c>
-      <c r="K21" t="n">
+      <c r="N21" t="n">
         <v>0.1185000017285347</v>
       </c>
-      <c r="L21" t="n">
+      <c r="O21" t="n">
         <v>0.005900000222027302</v>
       </c>
-      <c r="M21" t="n">
+      <c r="P21" t="n">
         <v>0.4752624034881592</v>
       </c>
-      <c r="N21" t="n">
+      <c r="Q21" t="n">
         <v>3.402863264083862</v>
       </c>
-      <c r="O21" t="n">
+      <c r="R21" t="n">
         <v>0.1185000017285347</v>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="S21" t="inlineStr">
         <is>
           <t>logs/results_126.log</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="T21" t="inlineStr">
         <is>
           <t>weights/model_126.ckpt</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr">
+      <c r="U21" t="inlineStr">
         <is>
           <t>tb/126/non_robust</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr">
+      <c r="V21" t="inlineStr">
         <is>
           <t>(0.90816385, 0.7060737, 0.9453165, 1.4311132, 1.8074349, 2.626249, 3.3506863)</t>
         </is>
       </c>
-      <c r="T21" t="inlineStr">
+      <c r="W21" t="inlineStr">
         <is>
           <t>(15.063638, 2.4488645, 2.8450708, 3.4224455, 2.870352, 2.775072, 2.7803397, 3.6928034)</t>
         </is>
@@ -1790,61 +1865,64 @@
       <c r="C22" t="n">
         <v>0</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
         <v>0.003</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11c4be9d8&gt;</t>
         </is>
       </c>
-      <c r="J22" t="n">
+      <c r="M22" t="n">
         <v>0.9559000134468079</v>
       </c>
-      <c r="K22" t="n">
+      <c r="N22" t="n">
         <v>0.05790000036358833</v>
       </c>
-      <c r="L22" t="n">
+      <c r="O22" t="n">
         <v>0.04890000075101852</v>
       </c>
-      <c r="M22" t="n">
+      <c r="P22" t="n">
         <v>0.1738029420375824</v>
       </c>
-      <c r="N22" t="n">
+      <c r="Q22" t="n">
         <v>6.665348529815674</v>
       </c>
-      <c r="O22" t="n">
+      <c r="R22" t="n">
         <v>0.05790000036358833</v>
       </c>
-      <c r="P22" t="inlineStr">
+      <c r="S22" t="inlineStr">
         <is>
           <t>logs/results_222.log</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="T22" t="inlineStr">
         <is>
           <t>weights/model_222.ckpt</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
+      <c r="U22" t="inlineStr">
         <is>
           <t>tb/222/non_robust</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
+      <c r="V22" t="inlineStr">
         <is>
           <t>(7.230026, 8.443772, 9.982576, 10.426454, 10.48337, 10.4655, 8.748777)</t>
         </is>
       </c>
-      <c r="T22" t="inlineStr">
+      <c r="W22" t="inlineStr">
         <is>
           <t>(139.92761, 9.773078, 8.607171, 8.341426, 7.4237742, 7.5570107, 6.5512905, 8.353663)</t>
         </is>
@@ -1860,61 +1938,64 @@
       <c r="C23" t="n">
         <v>0</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
         <v>0.003</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr">
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x11e21a9d8&gt;</t>
         </is>
       </c>
-      <c r="J23" t="n">
+      <c r="M23" t="n">
         <v>0.9312000274658203</v>
       </c>
-      <c r="K23" t="n">
+      <c r="N23" t="n">
         <v>0.06909999996423721</v>
       </c>
-      <c r="L23" t="n">
+      <c r="O23" t="n">
         <v>0.1206000000238419</v>
       </c>
-      <c r="M23" t="n">
+      <c r="P23" t="n">
         <v>0.2596416771411896</v>
       </c>
-      <c r="N23" t="n">
+      <c r="Q23" t="n">
         <v>7.456814289093018</v>
       </c>
-      <c r="O23" t="n">
+      <c r="R23" t="n">
         <v>0.06909999996423721</v>
       </c>
-      <c r="P23" t="inlineStr">
+      <c r="S23" t="inlineStr">
         <is>
           <t>logs/results_232.log</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
+      <c r="T23" t="inlineStr">
         <is>
           <t>weights/model_232.ckpt</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
+      <c r="U23" t="inlineStr">
         <is>
           <t>tb/232/non_robust</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
+      <c r="V23" t="inlineStr">
         <is>
           <t>(7.3609123, 7.8955326, 9.737668, 9.91078, 10.763038, 10.914308, 9.4478855)</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr">
+      <c r="W23" t="inlineStr">
         <is>
           <t>(140.87561, 8.819877, 8.838883, 8.998733, 7.921186, 7.691656, 7.321085, 9.176294)</t>
         </is>
@@ -1930,61 +2011,64 @@
       <c r="C24" t="n">
         <v>0</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
         <v>0.003</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr">
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x111a129d8&gt;</t>
         </is>
       </c>
-      <c r="J24" t="n">
+      <c r="M24" t="n">
         <v>0.9312999844551086</v>
       </c>
-      <c r="K24" t="n">
+      <c r="N24" t="n">
         <v>0.03830000013113022</v>
       </c>
-      <c r="L24" t="n">
+      <c r="O24" t="n">
         <v>0.009100000374019146</v>
       </c>
-      <c r="M24" t="n">
+      <c r="P24" t="n">
         <v>0.2439231872558594</v>
       </c>
-      <c r="N24" t="n">
+      <c r="Q24" t="n">
         <v>7.289804458618164</v>
       </c>
-      <c r="O24" t="n">
+      <c r="R24" t="n">
         <v>0.03830000013113022</v>
       </c>
-      <c r="P24" t="inlineStr">
+      <c r="S24" t="inlineStr">
         <is>
           <t>logs/results_234.log</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
+      <c r="T24" t="inlineStr">
         <is>
           <t>weights/model_234.ckpt</t>
         </is>
       </c>
-      <c r="R24" t="inlineStr">
+      <c r="U24" t="inlineStr">
         <is>
           <t>tb/234/non_robust</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="V24" t="inlineStr">
         <is>
           <t>(7.0172796, 7.6613173, 8.302304, 8.662146, 7.9462867, 9.3396435, 7.44935)</t>
         </is>
       </c>
-      <c r="T24" t="inlineStr">
+      <c r="W24" t="inlineStr">
         <is>
           <t>(136.32106, 9.159889, 8.33736, 8.452992, 7.9244547, 7.2932935, 7.7801814, 9.626968)</t>
         </is>
@@ -2000,63 +2084,66 @@
       <c r="C25" t="n">
         <v>0</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="n">
         <v>0.003</v>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>PGD</t>
         </is>
       </c>
-      <c r="F25" t="n">
+      <c r="I25" t="n">
         <v>0.1</v>
       </c>
-      <c r="G25" t="n">
+      <c r="J25" t="n">
         <v>0.1</v>
       </c>
-      <c r="H25" t="n">
+      <c r="K25" t="n">
         <v>3</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x118b969d8&gt;</t>
         </is>
       </c>
-      <c r="J25" t="n">
+      <c r="M25" t="n">
         <v>0.8787999749183655</v>
       </c>
-      <c r="K25" t="n">
+      <c r="N25" t="n">
         <v>0.01040000002831221</v>
       </c>
-      <c r="L25" t="n">
+      <c r="O25" t="n">
         <v>0.001300000003539026</v>
       </c>
-      <c r="M25" t="n">
+      <c r="P25" t="n">
         <v>0.4310351014137268</v>
       </c>
-      <c r="N25" t="n">
+      <c r="Q25" t="n">
         <v>8.296195983886719</v>
       </c>
-      <c r="O25" t="n">
+      <c r="R25" t="n">
         <v>0.01040000002831221</v>
       </c>
-      <c r="P25" t="inlineStr">
+      <c r="S25" t="inlineStr">
         <is>
           <t>logs/results_278.log</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="T25" t="inlineStr">
         <is>
           <t>weights/model_278.ckpt</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr">
+      <c r="U25" t="inlineStr">
         <is>
           <t>tb/278/robust</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2068,63 +2155,66 @@
       <c r="C26" t="n">
         <v>0</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="n">
         <v>0.003</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>PGD</t>
         </is>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
         <v>0.1</v>
       </c>
-      <c r="G26" t="n">
+      <c r="J26" t="n">
         <v>0.1</v>
       </c>
-      <c r="H26" t="n">
+      <c r="K26" t="n">
         <v>3</v>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x121b0f9d8&gt;</t>
         </is>
       </c>
-      <c r="J26" t="n">
+      <c r="M26" t="n">
         <v>0.8522999882698059</v>
       </c>
-      <c r="K26" t="n">
+      <c r="N26" t="n">
         <v>0.002899999963119626</v>
       </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
         <v>0.5192863941192627</v>
       </c>
-      <c r="N26" t="n">
+      <c r="Q26" t="n">
         <v>9.538139343261719</v>
       </c>
-      <c r="O26" t="n">
+      <c r="R26" t="n">
         <v>0.002899999963119626</v>
       </c>
-      <c r="P26" t="inlineStr">
+      <c r="S26" t="inlineStr">
         <is>
           <t>logs/results_279.log</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr">
+      <c r="T26" t="inlineStr">
         <is>
           <t>weights/model_279.ckpt</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr">
+      <c r="U26" t="inlineStr">
         <is>
           <t>tb/279/robust</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2136,63 +2226,66 @@
       <c r="C27" t="n">
         <v>0</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
         <v>0.003</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>PGD</t>
         </is>
       </c>
-      <c r="F27" t="n">
+      <c r="I27" t="n">
         <v>0.1</v>
       </c>
-      <c r="G27" t="n">
+      <c r="J27" t="n">
         <v>0.1</v>
       </c>
-      <c r="H27" t="n">
+      <c r="K27" t="n">
         <v>3</v>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x121b0f9d8&gt;</t>
         </is>
       </c>
-      <c r="J27" t="n">
+      <c r="M27" t="n">
         <v>0.8676999807357788</v>
       </c>
-      <c r="K27" t="n">
+      <c r="N27" t="n">
         <v>0.004999999888241291</v>
       </c>
-      <c r="L27" t="n">
+      <c r="O27" t="n">
         <v>9.999999747378752e-05</v>
       </c>
-      <c r="M27" t="n">
+      <c r="P27" t="n">
         <v>0.4790646433830261</v>
       </c>
-      <c r="N27" t="n">
+      <c r="Q27" t="n">
         <v>9.238405227661133</v>
       </c>
-      <c r="O27" t="n">
+      <c r="R27" t="n">
         <v>0.004999999888241291</v>
       </c>
-      <c r="P27" t="inlineStr">
+      <c r="S27" t="inlineStr">
         <is>
           <t>logs/results_279.log</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
+      <c r="T27" t="inlineStr">
         <is>
           <t>weights/model_279.ckpt</t>
         </is>
       </c>
-      <c r="R27" t="inlineStr">
+      <c r="U27" t="inlineStr">
         <is>
           <t>tb/279/robust</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2204,61 +2297,64 @@
       <c r="C28" t="n">
         <v>0</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="n">
         <v>0.003</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr">
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x10f4d69d8&gt;</t>
         </is>
       </c>
-      <c r="J28" t="n">
+      <c r="M28" t="n">
         <v>0.9516000151634216</v>
       </c>
-      <c r="K28" t="n">
+      <c r="N28" t="n">
         <v>0.04560000076889992</v>
       </c>
-      <c r="L28" t="n">
+      <c r="O28" t="n">
         <v>0.003700000001117587</v>
       </c>
-      <c r="M28" t="n">
+      <c r="P28" t="n">
         <v>0.1825118958950043</v>
       </c>
-      <c r="N28" t="n">
+      <c r="Q28" t="n">
         <v>6.906796932220459</v>
       </c>
-      <c r="O28" t="n">
+      <c r="R28" t="n">
         <v>0.04560000076889992</v>
       </c>
-      <c r="P28" t="inlineStr">
+      <c r="S28" t="inlineStr">
         <is>
           <t>logs/results_282.log</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr">
+      <c r="T28" t="inlineStr">
         <is>
           <t>weights/model_282.ckpt</t>
         </is>
       </c>
-      <c r="R28" t="inlineStr">
+      <c r="U28" t="inlineStr">
         <is>
           <t>tb/282</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr">
+      <c r="V28" t="inlineStr">
         <is>
           <t>(6.9546156, 7.3834124, 9.092276, 9.433221, 9.5498905, 11.14911, 9.904368)</t>
         </is>
       </c>
-      <c r="T28" t="inlineStr">
+      <c r="W28" t="inlineStr">
         <is>
           <t>(139.42224, 9.018682, 9.271418, 8.975029, 7.9992733, 7.393931, 7.053868, 10.015819)</t>
         </is>
@@ -2274,61 +2370,64 @@
       <c r="C29" t="n">
         <v>0</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="n">
         <v>0.003</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr">
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1100289d8&gt;</t>
         </is>
       </c>
-      <c r="J29" t="n">
+      <c r="M29" t="n">
         <v>0.9430999755859375</v>
       </c>
-      <c r="K29" t="n">
+      <c r="N29" t="n">
         <v>0.06279999762773514</v>
       </c>
-      <c r="L29" t="n">
+      <c r="O29" t="n">
         <v>0.006200000178068876</v>
       </c>
-      <c r="M29" t="n">
+      <c r="P29" t="n">
         <v>0.2192680686712265</v>
       </c>
-      <c r="N29" t="n">
+      <c r="Q29" t="n">
         <v>7.151318073272705</v>
       </c>
-      <c r="O29" t="n">
+      <c r="R29" t="n">
         <v>0.06279999762773514</v>
       </c>
-      <c r="P29" t="inlineStr">
+      <c r="S29" t="inlineStr">
         <is>
           <t>logs/results_285.log</t>
         </is>
       </c>
-      <c r="Q29" t="inlineStr">
+      <c r="T29" t="inlineStr">
         <is>
           <t>weights/model_285.ckpt</t>
         </is>
       </c>
-      <c r="R29" t="inlineStr">
+      <c r="U29" t="inlineStr">
         <is>
           <t>tb/285</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
+      <c r="V29" t="inlineStr">
         <is>
           <t>(7.0936155, 7.6124697, 8.267413, 8.219525, 11.057663, 10.19839, 9.6345)</t>
         </is>
       </c>
-      <c r="T29" t="inlineStr">
+      <c r="W29" t="inlineStr">
         <is>
           <t>(141.34113, 8.731318, 9.105043, 8.344593, 9.322138, 7.830576, 7.469233, 9.507704)</t>
         </is>
@@ -2344,61 +2443,64 @@
       <c r="C30" t="n">
         <v>0</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="n">
         <v>0.003</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr">
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x116aa89d8&gt;</t>
         </is>
       </c>
-      <c r="J30" t="n">
+      <c r="M30" t="n">
         <v>0.9474999904632568</v>
       </c>
-      <c r="K30" t="n">
+      <c r="N30" t="n">
         <v>0.07349999994039536</v>
       </c>
-      <c r="L30" t="n">
+      <c r="O30" t="n">
         <v>0.03050000034272671</v>
       </c>
-      <c r="M30" t="n">
+      <c r="P30" t="n">
         <v>0.2007102072238922</v>
       </c>
-      <c r="N30" t="n">
+      <c r="Q30" t="n">
         <v>6.25114631652832</v>
       </c>
-      <c r="O30" t="n">
+      <c r="R30" t="n">
         <v>0.07349999994039536</v>
       </c>
-      <c r="P30" t="inlineStr">
+      <c r="S30" t="inlineStr">
         <is>
           <t>logs/results_305.log</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr">
+      <c r="T30" t="inlineStr">
         <is>
           <t>weights/model_305.ckpt</t>
         </is>
       </c>
-      <c r="R30" t="inlineStr">
+      <c r="U30" t="inlineStr">
         <is>
           <t>tb/305</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
+      <c r="V30" t="inlineStr">
         <is>
           <t>(6.9461164, 7.606389, 7.896417, 8.789286, 9.165759, 8.689637, 8.321884)</t>
         </is>
       </c>
-      <c r="T30" t="inlineStr">
+      <c r="W30" t="inlineStr">
         <is>
           <t>(138.02159, 8.655811, 9.216804, 9.208384, 7.499287, 7.888038, 7.191258, 13.024145)</t>
         </is>
@@ -2414,61 +2516,64 @@
       <c r="C31" t="n">
         <v>0</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="n">
         <v>0.003</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>FGSM</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr">
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x128d789d8&gt;</t>
         </is>
       </c>
-      <c r="J31" t="n">
+      <c r="M31" t="n">
         <v>0.9329000115394592</v>
       </c>
-      <c r="K31" t="n">
+      <c r="N31" t="n">
         <v>0.7416999936103821</v>
       </c>
-      <c r="L31" t="n">
+      <c r="O31" t="n">
         <v>0.5971999764442444</v>
       </c>
-      <c r="M31" t="n">
+      <c r="P31" t="n">
         <v>0.2206476628780365</v>
       </c>
-      <c r="N31" t="n">
+      <c r="Q31" t="n">
         <v>0.74456787109375</v>
       </c>
-      <c r="O31" t="n">
+      <c r="R31" t="n">
         <v>0.7416999936103821</v>
       </c>
-      <c r="P31" t="inlineStr">
+      <c r="S31" t="inlineStr">
         <is>
           <t>logs/results_328.log</t>
         </is>
       </c>
-      <c r="Q31" t="inlineStr">
+      <c r="T31" t="inlineStr">
         <is>
           <t>weights/model_328.ckpt</t>
         </is>
       </c>
-      <c r="R31" t="inlineStr">
+      <c r="U31" t="inlineStr">
         <is>
           <t>tb/328</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
+      <c r="V31" t="inlineStr">
         <is>
           <t>(12.799518, 16.56418, 25.464622, 25.766693, 14.9766655, 6.904501, 3.7851212)</t>
         </is>
       </c>
-      <c r="T31" t="inlineStr">
+      <c r="W31" t="inlineStr">
         <is>
           <t>(309.03058, 13.829748, 16.421766, 12.924315, 13.326067, 11.006118, 10.691159, 13.276878)</t>
         </is>
@@ -2484,61 +2589,64 @@
       <c r="C32" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="n">
         <v>0.003</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr">
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x113fe39d8&gt;</t>
         </is>
       </c>
-      <c r="J32" t="n">
+      <c r="M32" t="n">
         <v>0.9472000002861023</v>
       </c>
-      <c r="K32" t="n">
+      <c r="N32" t="n">
         <v>0.3325000107288361</v>
       </c>
-      <c r="L32" t="n">
+      <c r="O32" t="n">
         <v>0.1923000067472458</v>
       </c>
-      <c r="M32" t="n">
+      <c r="P32" t="n">
         <v>0.1799724549055099</v>
       </c>
-      <c r="N32" t="n">
+      <c r="Q32" t="n">
         <v>3.20237398147583</v>
       </c>
-      <c r="O32" t="n">
+      <c r="R32" t="n">
         <v>0.3325000107288361</v>
       </c>
-      <c r="P32" t="inlineStr">
+      <c r="S32" t="inlineStr">
         <is>
           <t>logs/results_331.log</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
+      <c r="T32" t="inlineStr">
         <is>
           <t>weights/model_331.ckpt</t>
         </is>
       </c>
-      <c r="R32" t="inlineStr">
+      <c r="U32" t="inlineStr">
         <is>
           <t>tb/331</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr">
+      <c r="V32" t="inlineStr">
         <is>
           <t>(1.8040013, 1.8094578, 1.9554862, 2.5528448, 3.399231, 4.635884, 6.39143)</t>
         </is>
       </c>
-      <c r="T32" t="inlineStr">
+      <c r="W32" t="inlineStr">
         <is>
           <t>(28.089184, 4.674623, 3.6114936, 3.2815678, 3.1776936, 2.116904, 2.2179012, 2.6026235)</t>
         </is>
@@ -2554,61 +2662,64 @@
       <c r="C33" t="n">
         <v>0.0009</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="n">
         <v>0.003</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr">
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x118f1b9d8&gt;</t>
         </is>
       </c>
-      <c r="J33" t="n">
+      <c r="M33" t="n">
         <v>0.8956000208854675</v>
       </c>
-      <c r="K33" t="n">
+      <c r="N33" t="n">
         <v>0.3217999935150146</v>
       </c>
-      <c r="L33" t="n">
+      <c r="O33" t="n">
         <v>0.2044000029563904</v>
       </c>
-      <c r="M33" t="n">
+      <c r="P33" t="n">
         <v>0.3738516569137573</v>
       </c>
-      <c r="N33" t="n">
+      <c r="Q33" t="n">
         <v>3.476548433303833</v>
       </c>
-      <c r="O33" t="n">
+      <c r="R33" t="n">
         <v>0.3217999935150146</v>
       </c>
-      <c r="P33" t="inlineStr">
+      <c r="S33" t="inlineStr">
         <is>
           <t>logs/results_332.log</t>
         </is>
       </c>
-      <c r="Q33" t="inlineStr">
+      <c r="T33" t="inlineStr">
         <is>
           <t>weights/model_332.ckpt</t>
         </is>
       </c>
-      <c r="R33" t="inlineStr">
+      <c r="U33" t="inlineStr">
         <is>
           <t>tb/332</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
+      <c r="V33" t="inlineStr">
         <is>
           <t>(1.4544966, 1.1530415, 1.2943891, 2.1282125, 4.040144, 7.1142826, 6.1251535)</t>
         </is>
       </c>
-      <c r="T33" t="inlineStr">
+      <c r="W33" t="inlineStr">
         <is>
           <t>(21.872171, 4.500764, 3.899859, 2.0486226, 2.4281611, 2.2534535, 1.7587844, 2.4474022)</t>
         </is>
@@ -2624,61 +2735,64 @@
       <c r="C34" t="n">
         <v>0.0015</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr">
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x10b0f09d8&gt;</t>
         </is>
       </c>
-      <c r="J34" t="n">
+      <c r="M34" t="n">
         <v>0.9347000122070312</v>
       </c>
-      <c r="K34" t="n">
+      <c r="N34" t="n">
         <v>0.2572999894618988</v>
       </c>
-      <c r="L34" t="n">
+      <c r="O34" t="n">
         <v>0.1509999930858612</v>
       </c>
-      <c r="M34" t="n">
+      <c r="P34" t="n">
         <v>0.2364677786827087</v>
       </c>
-      <c r="N34" t="n">
+      <c r="Q34" t="n">
         <v>4.247204780578613</v>
       </c>
-      <c r="O34" t="n">
+      <c r="R34" t="n">
         <v>0.2572999894618988</v>
       </c>
-      <c r="P34" t="inlineStr">
+      <c r="S34" t="inlineStr">
         <is>
           <t>logs/results_333.log</t>
         </is>
       </c>
-      <c r="Q34" t="inlineStr">
+      <c r="T34" t="inlineStr">
         <is>
           <t>weights/model_333.ckpt</t>
         </is>
       </c>
-      <c r="R34" t="inlineStr">
+      <c r="U34" t="inlineStr">
         <is>
           <t>tb/333</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr">
+      <c r="V34" t="inlineStr">
         <is>
           <t>(0.4250503, 0.4371529, 0.74407357, 1.2906153, 2.5302472, 4.9194384, 6.6656017)</t>
         </is>
       </c>
-      <c r="T34" t="inlineStr">
+      <c r="W34" t="inlineStr">
         <is>
           <t>(6.92537, 5.7589846, 3.67073, 3.039194, 3.1920185, 5.1396704, 3.4247825, 4.5205474)</t>
         </is>
@@ -2694,61 +2808,64 @@
       <c r="C35" t="n">
         <v>1.5e-05</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr">
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1113b09d8&gt;</t>
         </is>
       </c>
-      <c r="J35" t="n">
+      <c r="M35" t="n">
         <v>0.9394999742507935</v>
       </c>
-      <c r="K35" t="n">
+      <c r="N35" t="n">
         <v>0.09109999984502792</v>
       </c>
-      <c r="L35" t="n">
+      <c r="O35" t="n">
         <v>0.03319999948143959</v>
       </c>
-      <c r="M35" t="n">
+      <c r="P35" t="n">
         <v>0.221238300204277</v>
       </c>
-      <c r="N35" t="n">
+      <c r="Q35" t="n">
         <v>6.377280712127686</v>
       </c>
-      <c r="O35" t="n">
+      <c r="R35" t="n">
         <v>0.09109999984502792</v>
       </c>
-      <c r="P35" t="inlineStr">
+      <c r="S35" t="inlineStr">
         <is>
           <t>logs/results_336.log</t>
         </is>
       </c>
-      <c r="Q35" t="inlineStr">
+      <c r="T35" t="inlineStr">
         <is>
           <t>weights/model_336.ckpt</t>
         </is>
       </c>
-      <c r="R35" t="inlineStr">
+      <c r="U35" t="inlineStr">
         <is>
           <t>tb/336</t>
         </is>
       </c>
-      <c r="S35" t="inlineStr">
+      <c r="V35" t="inlineStr">
         <is>
           <t>(2.0724185, 1.3095005, 1.6185311, 1.3509899, 1.5398465, 1.9591715, 4.275175)</t>
         </is>
       </c>
-      <c r="T35" t="inlineStr">
+      <c r="W35" t="inlineStr">
         <is>
           <t>(39.100674, 3.319005, 3.0519383, 1.6382135, 2.70516, 2.7627785, 5.8854613, 6.491546)</t>
         </is>
@@ -2764,61 +2881,64 @@
       <c r="C36" t="n">
         <v>2.3e-05</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr">
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1132949d8&gt;</t>
         </is>
       </c>
-      <c r="J36" t="n">
+      <c r="M36" t="n">
         <v>0.9189000129699707</v>
       </c>
-      <c r="K36" t="n">
+      <c r="N36" t="n">
         <v>0.05869999900460243</v>
       </c>
-      <c r="L36" t="n">
+      <c r="O36" t="n">
         <v>0.02209999971091747</v>
       </c>
-      <c r="M36" t="n">
+      <c r="P36" t="n">
         <v>0.3333184719085693</v>
       </c>
-      <c r="N36" t="n">
+      <c r="Q36" t="n">
         <v>6.367059707641602</v>
       </c>
-      <c r="O36" t="n">
+      <c r="R36" t="n">
         <v>0.05869999900460243</v>
       </c>
-      <c r="P36" t="inlineStr">
+      <c r="S36" t="inlineStr">
         <is>
           <t>logs/results_346.log</t>
         </is>
       </c>
-      <c r="Q36" t="inlineStr">
+      <c r="T36" t="inlineStr">
         <is>
           <t>weights/model_346.ckpt</t>
         </is>
       </c>
-      <c r="R36" t="inlineStr">
+      <c r="U36" t="inlineStr">
         <is>
           <t>tb/346</t>
         </is>
       </c>
-      <c r="S36" t="inlineStr">
+      <c r="V36" t="inlineStr">
         <is>
           <t>(1.5257524, 0.7150309, 0.56886697, 0.49205807, 0.57274866, 1.5198021, 4.5895967)</t>
         </is>
       </c>
-      <c r="T36" t="inlineStr">
+      <c r="W36" t="inlineStr">
         <is>
           <t>(33.718807, 2.9477801, 2.0959005, 1.7632871, 2.2024982, 4.748903, 8.546004, 6.910356)</t>
         </is>
@@ -2834,61 +2954,64 @@
       <c r="C37" t="n">
         <v>0.007</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr">
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1226c79d8&gt;</t>
         </is>
       </c>
-      <c r="J37" t="n">
+      <c r="M37" t="n">
         <v>0.9646999835968018</v>
       </c>
-      <c r="K37" t="n">
+      <c r="N37" t="n">
         <v>0.1290999948978424</v>
       </c>
-      <c r="L37" t="n">
+      <c r="O37" t="n">
         <v>0.01889999955892563</v>
       </c>
-      <c r="M37" t="n">
+      <c r="P37" t="n">
         <v>0.1261469274759293</v>
       </c>
-      <c r="N37" t="n">
+      <c r="Q37" t="n">
         <v>6.858481407165527</v>
       </c>
-      <c r="O37" t="n">
+      <c r="R37" t="n">
         <v>0.1290999948978424</v>
       </c>
-      <c r="P37" t="inlineStr">
+      <c r="S37" t="inlineStr">
         <is>
           <t>logs/results_353.log</t>
         </is>
       </c>
-      <c r="Q37" t="inlineStr">
+      <c r="T37" t="inlineStr">
         <is>
           <t>weights/model_353.ckpt</t>
         </is>
       </c>
-      <c r="R37" t="inlineStr">
+      <c r="U37" t="inlineStr">
         <is>
           <t>tb/353</t>
         </is>
       </c>
-      <c r="S37" t="inlineStr">
+      <c r="V37" t="inlineStr">
         <is>
           <t>(0.6469947, 0.73037505, 0.9719021, 1.3849623, 2.158197, 3.6967816, 6.6338224)</t>
         </is>
       </c>
-      <c r="T37" t="inlineStr">
+      <c r="W37" t="inlineStr">
         <is>
           <t>(9.72191, 3.5845523, 3.115291, 2.8329852, 2.7452235, 2.6821659, 2.723758, 2.6171021)</t>
         </is>
@@ -2904,65 +3027,422 @@
       <c r="C38" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr">
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr">
         <is>
           <t>&lt;function relu at 0x1226499d8&gt;</t>
         </is>
       </c>
-      <c r="J38" t="n">
+      <c r="M38" t="n">
         <v>0.9384999871253967</v>
       </c>
-      <c r="K38" t="n">
+      <c r="N38" t="n">
         <v>0.3431999981403351</v>
       </c>
-      <c r="L38" t="n">
+      <c r="O38" t="n">
         <v>0.217399999499321</v>
       </c>
-      <c r="M38" t="n">
+      <c r="P38" t="n">
         <v>0.2118040025234222</v>
       </c>
-      <c r="N38" t="n">
+      <c r="Q38" t="n">
         <v>2.253601551055908</v>
       </c>
-      <c r="O38" t="n">
+      <c r="R38" t="n">
         <v>0.3431999981403351</v>
       </c>
-      <c r="P38" t="inlineStr">
+      <c r="S38" t="inlineStr">
         <is>
           <t>logs/results_354.log</t>
         </is>
       </c>
-      <c r="Q38" t="inlineStr">
+      <c r="T38" t="inlineStr">
         <is>
           <t>weights/model_354.ckpt</t>
         </is>
       </c>
-      <c r="R38" t="inlineStr">
+      <c r="U38" t="inlineStr">
         <is>
           <t>tb/354</t>
         </is>
       </c>
-      <c r="S38" t="inlineStr">
+      <c r="V38" t="inlineStr">
         <is>
           <t>(0.2376155, 0.2859654, 0.43169716, 0.67097735, 1.0554945, 1.7692584, 2.8368058)</t>
         </is>
       </c>
-      <c r="T38" t="inlineStr">
+      <c r="W38" t="inlineStr">
         <is>
           <t>(3.0683854, 1.7650508, 1.7416625, 1.7273158, 1.7367424, 1.746138, 1.7387878, 1.7745363)</t>
         </is>
       </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>30</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x121d289d8&gt;</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>0.9521999955177307</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.1439999938011169</v>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="n">
+        <v>0.1563661247491837</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>5.463603973388672</v>
+      </c>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>weights/model_368.ckpt</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>100</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x121d289d8&gt;</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>0.9409000277519226</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.2567999958992004</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="n">
+        <v>0.1994846016168594</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>2.769212007522583</v>
+      </c>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>weights/model_369.ckpt</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>30</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x121d289d8&gt;</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>0.9591000080108643</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.2443999946117401</v>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="n">
+        <v>0.1414018124341965</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>4.95952844619751</v>
+      </c>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>weights/model_370.ckpt</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>30</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x121d289d8&gt;</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>0.8744999766349792</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.1708000004291534</v>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="n">
+        <v>0.4795523583889008</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>3.317811727523804</v>
+      </c>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>weights/model_371.ckpt</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>30</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11d707488&gt;</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>0.9039999842643738</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.3244999945163727</v>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="n">
+        <v>0.3338456153869629</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>3.569289922714233</v>
+      </c>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>weights/model_367.ckpt</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>30</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11d707488&gt;</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>0.9429000020027161</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.2337000072002411</v>
+      </c>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="n">
+        <v>0.1914694607257843</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>4.124828815460205</v>
+      </c>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>weights/model_367.ckpt</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Added new models to train many script and added complexity bounds
</commit_message>
<xml_diff>
--- a/scripts/results.xlsx
+++ b/scripts/results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W50"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3798,6 +3798,120 @@
       <c r="V50" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
     </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>10</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11d707488&gt;</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
+        <v>0.9351999759674072</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.3497999906539917</v>
+      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="n">
+        <v>0.2422611862421036</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>3.15626335144043</v>
+      </c>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>30</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Regular</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>&lt;function relu at 0x11d707488&gt;</t>
+        </is>
+      </c>
+      <c r="M52" t="n">
+        <v>0.9556999802589417</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.04399999976158142</v>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="n">
+        <v>0.2216933816671371</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>23.85161018371582</v>
+      </c>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>weights/model_367.ckpt</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>